<commit_message>
urls for aqua and cop3
</commit_message>
<xml_diff>
--- a/docs/quality_questions_excel_template.xlsx
+++ b/docs/quality_questions_excel_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repositories\analysis_project_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06D2EAAA-CD06-4985-B939-5FADAC67C247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A64A934C-3CEE-47DC-89D7-E4B75290C366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4FDAA091-8849-4C6D-BF6B-DA0083E52E8E}"/>
+    <workbookView xWindow="888" yWindow="972" windowWidth="21624" windowHeight="11244" activeTab="3" xr2:uid="{4FDAA091-8849-4C6D-BF6B-DA0083E52E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -3248,7 +3248,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3407,6 +3407,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -3894,7 +3902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4181,6 +4189,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5992,25 +6003,25 @@
       <c r="B4" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="110"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="111"/>
     </row>
     <row r="5" spans="1:156" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="110"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="111"/>
     </row>
     <row r="6" spans="1:156" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="110"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="111"/>
       <c r="F6" s="48" t="s">
         <v>64</v>
       </c>
@@ -6019,9 +6030,9 @@
       <c r="B7" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="110"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="111"/>
       <c r="F7" s="48" t="s">
         <v>66</v>
       </c>
@@ -6030,17 +6041,17 @@
       <c r="B8" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="110"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="111"/>
     </row>
     <row r="9" spans="1:156" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="48" t="s">
         <v>69</v>
       </c>
@@ -6049,17 +6060,17 @@
       <c r="B10" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="110"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="111"/>
     </row>
     <row r="11" spans="1:156" ht="45" x14ac:dyDescent="0.2">
       <c r="B11" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="110"/>
+      <c r="C11" s="109"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="48" t="s">
         <v>72</v>
       </c>
@@ -6068,9 +6079,9 @@
       <c r="B12" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="110"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
     </row>
     <row r="13" spans="1:156" x14ac:dyDescent="0.2">
       <c r="B13" s="43"/>
@@ -6094,10 +6105,10 @@
       <c r="C15" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="112"/>
+      <c r="E15" s="113"/>
       <c r="F15" s="52" t="s">
         <v>78</v>
       </c>
@@ -6107,8 +6118,8 @@
         <v>201</v>
       </c>
       <c r="C16" s="54"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="115"/>
       <c r="F16" s="48" t="s">
         <v>79</v>
       </c>
@@ -6118,16 +6129,16 @@
         <v>80</v>
       </c>
       <c r="C17" s="55"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="110"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="111"/>
     </row>
     <row r="18" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="56" t="s">
         <v>202</v>
       </c>
       <c r="C18" s="57"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="110"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="111"/>
       <c r="F18" s="48" t="s">
         <v>81</v>
       </c>
@@ -6137,8 +6148,8 @@
         <v>82</v>
       </c>
       <c r="C19" s="57"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="110"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="111"/>
       <c r="F19" s="48" t="s">
         <v>81</v>
       </c>
@@ -6175,33 +6186,33 @@
       <c r="B25" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="105"/>
-      <c r="D25" s="115"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="116"/>
       <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="105"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="107"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="108"/>
     </row>
     <row r="27" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="107"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="107"/>
+      <c r="E27" s="108"/>
     </row>
     <row r="28" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="105"/>
-      <c r="D28" s="106"/>
-      <c r="E28" s="107"/>
+      <c r="C28" s="106"/>
+      <c r="D28" s="107"/>
+      <c r="E28" s="108"/>
     </row>
     <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A32" s="45" t="s">
@@ -6305,7 +6316,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6333,13 +6344,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="65" customFormat="1" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
       <c r="F1" s="43"/>
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
@@ -6348,19 +6359,19 @@
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
       <c r="M1" s="43"/>
-      <c r="N1" s="118" t="s">
+      <c r="N1" s="119" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="121"/>
     </row>
     <row r="2" spans="1:21" s="66" customFormat="1" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="105" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="86" t="s">
@@ -6369,10 +6380,10 @@
       <c r="C2" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="105" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="86" t="s">
+      <c r="E2" s="105" t="s">
         <v>98</v>
       </c>
       <c r="F2" s="87" t="s">
@@ -6425,7 +6436,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="122" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="91">
@@ -6478,7 +6489,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121"/>
+      <c r="A4" s="122"/>
       <c r="B4" s="92">
         <f>B3+1</f>
         <v>2</v>
@@ -6528,7 +6539,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="121"/>
+      <c r="A5" s="122"/>
       <c r="B5" s="92">
         <f t="shared" ref="B5:B21" si="0">B4+1</f>
         <v>3</v>
@@ -6576,7 +6587,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="92">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6624,7 +6635,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="92">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6674,7 +6685,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="92">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6722,7 +6733,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="121"/>
+      <c r="A9" s="122"/>
       <c r="B9" s="92">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6772,7 +6783,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="92">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6822,7 +6833,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121"/>
+      <c r="A11" s="122"/>
       <c r="B11" s="92">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6870,7 +6881,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
+      <c r="A12" s="122"/>
       <c r="B12" s="92">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6918,7 +6929,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="121"/>
+      <c r="A13" s="122"/>
       <c r="B13" s="92">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6966,7 +6977,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="121"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="92">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7016,7 +7027,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="121"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="92">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7064,7 +7075,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="121"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="92">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7114,7 +7125,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="121"/>
+      <c r="A17" s="122"/>
       <c r="B17" s="92">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7162,7 +7173,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="121"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="92">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7210,7 +7221,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="38.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="121"/>
+      <c r="A19" s="122"/>
       <c r="B19" s="92">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7258,7 +7269,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="92">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7306,7 +7317,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="121"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="92">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7356,7 +7367,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="122" t="s">
+      <c r="A22" s="123" t="s">
         <v>136</v>
       </c>
       <c r="B22" s="93">
@@ -7406,7 +7417,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="93">
         <f t="shared" ref="B23:B27" si="1">B22+1</f>
         <v>21</v>
@@ -7458,7 +7469,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
+      <c r="A24" s="123"/>
       <c r="B24" s="93">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -7508,7 +7519,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="93">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -7558,7 +7569,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="93">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -7610,7 +7621,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
+      <c r="A27" s="123"/>
       <c r="B27" s="93">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -7660,7 +7671,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="123" t="s">
+      <c r="A28" s="124" t="s">
         <v>200</v>
       </c>
       <c r="B28" s="94">
@@ -7710,7 +7721,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="123"/>
+      <c r="A29" s="124"/>
       <c r="B29" s="94">
         <f t="shared" ref="B29:B54" si="2">B28+1</f>
         <v>27</v>
@@ -7758,7 +7769,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="123"/>
+      <c r="A30" s="124"/>
       <c r="B30" s="94">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -7808,7 +7819,7 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="94">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -7858,7 +7869,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="123"/>
+      <c r="A32" s="124"/>
       <c r="B32" s="94">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -7906,7 +7917,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="123"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="94">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -7956,7 +7967,7 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="123"/>
+      <c r="A34" s="124"/>
       <c r="B34" s="94">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -8006,7 +8017,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="123"/>
+      <c r="A35" s="124"/>
       <c r="B35" s="94">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -8056,7 +8067,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="123"/>
+      <c r="A36" s="124"/>
       <c r="B36" s="94">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -8106,7 +8117,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="124"/>
+      <c r="A37" s="125"/>
       <c r="B37" s="94">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -8156,7 +8167,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="124"/>
+      <c r="A38" s="125"/>
       <c r="B38" s="94">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -8204,7 +8215,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="124"/>
+      <c r="A39" s="125"/>
       <c r="B39" s="94">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -8256,7 +8267,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="124"/>
+      <c r="A40" s="125"/>
       <c r="B40" s="94">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -8304,7 +8315,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="124"/>
+      <c r="A41" s="125"/>
       <c r="B41" s="94">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -8352,7 +8363,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="124"/>
+      <c r="A42" s="125"/>
       <c r="B42" s="94">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8402,7 +8413,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="124"/>
+      <c r="A43" s="125"/>
       <c r="B43" s="94">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -8450,7 +8461,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="124"/>
+      <c r="A44" s="125"/>
       <c r="B44" s="94">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8498,7 +8509,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="124"/>
+      <c r="A45" s="125"/>
       <c r="B45" s="94">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -8546,7 +8557,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="124"/>
+      <c r="A46" s="125"/>
       <c r="B46" s="94">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8594,7 +8605,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="124"/>
+      <c r="A47" s="125"/>
       <c r="B47" s="94">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -8644,7 +8655,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="124"/>
+      <c r="A48" s="125"/>
       <c r="B48" s="94">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -8696,7 +8707,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="124"/>
+      <c r="A49" s="125"/>
       <c r="B49" s="94">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -8748,7 +8759,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="124"/>
+      <c r="A50" s="125"/>
       <c r="B50" s="94">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -8798,7 +8809,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="124"/>
+      <c r="A51" s="125"/>
       <c r="B51" s="94">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -8848,7 +8859,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="124"/>
+      <c r="A52" s="125"/>
       <c r="B52" s="94">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -8898,7 +8909,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="124"/>
+      <c r="A53" s="125"/>
       <c r="B53" s="94">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -8946,7 +8957,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="124"/>
+      <c r="A54" s="125"/>
       <c r="B54" s="94">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -8996,7 +9007,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="116" t="s">
+      <c r="A55" s="117" t="s">
         <v>173</v>
       </c>
       <c r="B55" s="95">
@@ -9050,7 +9061,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="116"/>
+      <c r="A56" s="117"/>
       <c r="B56" s="95">
         <f t="shared" ref="B56:B63" si="3">B55+1</f>
         <v>54</v>
@@ -9102,7 +9113,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
+      <c r="A57" s="117"/>
       <c r="B57" s="95">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -9150,7 +9161,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="116"/>
+      <c r="A58" s="117"/>
       <c r="B58" s="95">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -9198,7 +9209,7 @@
       </c>
     </row>
     <row r="59" spans="1:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="116"/>
+      <c r="A59" s="117"/>
       <c r="B59" s="95">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -9246,7 +9257,7 @@
       </c>
     </row>
     <row r="60" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="116"/>
+      <c r="A60" s="117"/>
       <c r="B60" s="95">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -9294,7 +9305,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
+      <c r="A61" s="117"/>
       <c r="B61" s="95">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -9344,7 +9355,7 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="116"/>
+      <c r="A62" s="117"/>
       <c r="B62" s="95">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -9392,7 +9403,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="116"/>
+      <c r="A63" s="117"/>
       <c r="B63" s="95">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -9507,7 +9518,7 @@
       <c r="A73" s="81"/>
     </row>
   </sheetData>
-  <sheetProtection autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="s7nAzo09W2pu2pzQxulB3LlOS7rHZ4SsWO15JFaLskelUu/GN7QvvgWkUmZOUd2ZxrR+liz7CdBg0GlznXakLg==" saltValue="Rbqp9J6mh5Kr1vIR14BXeQ==" spinCount="100000" sheet="1" autoFilter="0"/>
   <autoFilter ref="A2:U65" xr:uid="{40CE4B58-4DDE-4FFB-AF5D-92EC82F1F313}"/>
   <mergeCells count="6">
     <mergeCell ref="A55:A63"/>
@@ -9526,37 +9537,20 @@
     <hyperlink ref="N1:U1" r:id="rId1" display="ONS Quality Standard for Analysis Phases (mapping to QQ)" xr:uid="{738D2B97-F3BD-4FDE-8272-ABCE9901DFFB}"/>
     <hyperlink ref="L2" r:id="rId2" display="Analysis Function Guidance (Quality Q and Red F)" xr:uid="{C326AE48-58B3-4656-A65A-B2EA8649E904}"/>
     <hyperlink ref="M2" r:id="rId3" display="OSR Guidance" xr:uid="{5BA16752-6848-4CA7-8FA9-C75C10775F25}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{DC07AB57-F3D3-4D54-8EDC-B61894755AC9}"/>
+    <hyperlink ref="A2" r:id="rId5" location="roles" xr:uid="{095F8ED3-C96B-4E3C-ACB9-7B45814E01A1}"/>
+    <hyperlink ref="E2" r:id="rId6" location="roles" xr:uid="{03048F9D-EB72-4350-8A41-0769749E87F0}"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="44" fitToWidth="2" fitToHeight="3" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="44" fitToWidth="2" fitToHeight="3" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId7"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="21" max="16383" man="1"/>
   </rowBreaks>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031C6D98A8BA9914F9CBD1D8D43561C2B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3360ac36c85262295d12999d22c2e363">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e1cd103-0302-4a32-9a4b-e115c950d959" xmlns:ns3="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb3c89d64baff4fee9c4315563c133e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
@@ -9805,32 +9799,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85AF8313-FA00-4D59-B28F-14781BE72D64}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A7238D-7DAD-4EFF-B184-28E2DF4DDCD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E2C66AF-212F-4C93-99E0-4ABA57FC8364}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9849,6 +9838,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85AF8313-FA00-4D59-B28F-14781BE72D64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A7238D-7DAD-4EFF-B184-28E2DF4DDCD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{078807bf-ce82-4688-bce0-0d811684dc46}" enabled="0" method="" siteId="{078807bf-ce82-4688-bce0-0d811684dc46}" removed="1"/>

</xml_diff>

<commit_message>
updating excel template for aqua role descriptions
</commit_message>
<xml_diff>
--- a/docs/quality_questions_excel_template.xlsx
+++ b/docs/quality_questions_excel_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repositories\analysis_project_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A64A934C-3CEE-47DC-89D7-E4B75290C366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{276B85AB-C49F-49CE-AF0C-2CD09A945641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="972" windowWidth="21624" windowHeight="11244" activeTab="3" xr2:uid="{4FDAA091-8849-4C6D-BF6B-DA0083E52E8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4FDAA091-8849-4C6D-BF6B-DA0083E52E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -49,167 +49,107 @@
   <authors>
     <author>tc={7F5710BC-5B55-4CAE-8B89-547AD4B6D83A}</author>
     <author>Note</author>
-    <author>tc={E21B303B-A7CD-43D0-B7EA-D905F032D9A5}</author>
+    <author>Copilot</author>
     <author>tc={B717D9AE-0604-44A0-8412-B2D09E13C4CC}</author>
     <author>tc={47B98FA1-7526-49B8-89A9-EF77BCA91D0E}</author>
     <author>tc={613A47E9-079E-4E6B-8BDB-20CC09BE4753}</author>
-    <author>tc={493BD2CC-B01C-4431-A4D3-5FF34D608502}</author>
     <author>tc={9CF26141-1975-4AF9-A051-D7457E18733E}</author>
     <author>tc={ECE1C9BD-0F1F-48B0-8E29-32AEC4DC9500}</author>
-    <author>tc={87ABBA1D-1BFB-4597-950F-7EA7A2EF80B2}</author>
     <author>tc={FDBC8216-3E37-4E41-BCE3-4BA3377DA5C0}</author>
-    <author>tc={8EB3435E-2AD8-4AF9-9477-10355940958D}</author>
     <author>tc={BCCD1820-2B3B-4FEC-8B83-86DBCC941395}</author>
-    <author>tc={18A1EB84-066B-483A-A278-351D641106BE}</author>
     <author>tc={BC3B8A1E-E152-4A66-BD49-D05803E09CA5}</author>
     <author>tc={FB0F022A-E355-466D-8B31-2880B5FA0755}</author>
-    <author>tc={AA6BAEC1-9530-43AE-A233-E2E7C0374046}</author>
     <author>tc={FB4107FF-85E4-4674-9C4E-7753AB019F16}</author>
-    <author>tc={EF364E4F-6B64-4BFB-8A60-041DE12319C2}</author>
     <author>tc={4D792EE8-5DFC-473C-9F60-5F342A95B67E}</author>
     <author>tc={8FABEAEF-BAE0-4A77-A3E0-5BF27B3BD2A3}</author>
-    <author>tc={4A376BBA-7716-405F-A998-FBDCCFB6D36A}</author>
     <author>tc={297D13ED-C651-43E5-A296-C92BDF8140A0}</author>
     <author>tc={B8611E4F-62CB-4E5B-B541-B7D57EDFE31B}</author>
-    <author>tc={91DA7871-3F83-489C-9B2C-D097153E5C8B}</author>
     <author>tc={DDA67DCB-8363-4F2A-8E2F-D7FD31758CC8}</author>
-    <author>tc={0229EB7C-8A73-4B9E-9D13-796DEAA70543}</author>
     <author>tc={4EFF044A-661A-45F8-9173-7EAF843C1921}</author>
-    <author>tc={0B3233E4-B736-4C2D-AADA-A0925FF322D3}</author>
     <author>tc={B074A2B9-B46E-4830-BCD5-A7D9FC9F80B3}</author>
-    <author>tc={F49D43AA-2830-4C6A-B1BB-5F30B710381C}</author>
     <author>tc={14C4500A-297B-4DC2-A81E-5404A0E6855E}</author>
     <author>tc={BDD5D421-F6F7-4018-BBB9-CC062F53505D}</author>
-    <author>tc={A8911257-2BC7-4D42-BB6B-8A505C0946B1}</author>
     <author>tc={675351E7-4AAD-4CAE-A63B-A1432693D85A}</author>
-    <author>tc={16B73972-A012-48B7-A793-DAD887DBB3BF}</author>
     <author>tc={247C10C3-5E6D-4D86-B576-9EA0227FA976}</author>
     <author>tc={8ACF04DB-3056-4F30-B39E-A41DFC39BAD7}</author>
-    <author>tc={38227814-F8B1-46EF-ABEB-7DEC64C60144}</author>
     <author>tc={59656D8A-69E5-4CDB-8CA0-48493A72EB6E}</author>
-    <author>tc={65E6E0EC-BC6A-4935-A14C-FBA6D651D1C0}</author>
     <author>tc={6326AB4D-3C57-460D-B340-3271BFEA81A2}</author>
-    <author>tc={E0E21280-EAE1-4A23-948F-48D7D64315E4}</author>
     <author>tc={C2A9A967-BCAA-453B-9DE1-A1889DA749F8}</author>
-    <author>tc={5BC7BB64-C399-4C88-910A-EE0A196D541B}</author>
     <author>tc={71D7AD01-61DA-4F82-B9B6-13FA8081889E}</author>
-    <author>tc={94791D6F-A09E-4058-A847-C891B2C626C4}</author>
     <author>tc={2711FEBA-50F1-49C4-BBCD-00FD8773322F}</author>
     <author>tc={C9BBB705-34D0-4287-A9AF-3DC9914279E0}</author>
-    <author>tc={816A930F-38AC-4BF9-B788-9577B0D60F19}</author>
     <author>tc={1F0E8DDD-3806-4EB2-A559-E138AD955876}</author>
-    <author>tc={13E8362D-B596-42DC-A9CB-A062A4B94158}</author>
     <author>tc={5EB69C75-C40A-4B3C-A1C9-C76AB1F55EF6}</author>
     <author>tc={E96E4235-11DB-49F7-9E37-142BBEE9E7C0}</author>
     <author>tc={41BE326F-BE7B-4F34-83F1-BA0897CC104B}</author>
-    <author>tc={278AF0F5-1106-492A-AB60-8B0CBF7DA4D5}</author>
     <author>tc={CF291131-C014-40E1-8BDC-CE14CA286B85}</author>
     <author>tc={76246FCF-D76F-44ED-98BE-AD6F708D60CB}</author>
-    <author>tc={A8AE3539-0828-48D7-85A6-95E81786F997}</author>
     <author>tc={75DDAEFF-7FE9-48F4-B766-4CAA33B2B677}</author>
     <author>tc={0CB30745-6A5E-4281-A26B-58CB004C625C}</author>
-    <author>tc={A42575B9-C972-453B-8A32-9A671BEDE603}</author>
     <author>tc={A312EA72-F9CB-4C05-8E8D-7D66458CCD38}</author>
     <author>tc={C78A230B-40F6-4C27-8D15-D5BF92F125EC}</author>
     <author>tc={394075A5-D7F4-4823-90DE-F6DAF78C70F5}</author>
-    <author>tc={FF90D25A-4F6A-4F0E-A1D7-85C575ABF4CF}</author>
     <author>tc={8680581D-D8CB-43C2-9441-DEA37E980EB7}</author>
     <author>tc={D988F73F-692A-43EF-A4EA-3CD1684C9B6D}</author>
-    <author>tc={1B01FECE-7BE0-4343-BCCC-DAEB90C40E6F}</author>
     <author>tc={1F976AE5-334F-44B3-8203-575633C5DBA1}</author>
-    <author>tc={33FFCD26-892E-48CB-9570-5772ACF052DA}</author>
     <author>tc={AE45F985-AF8D-42E4-9B36-D04CCB025BDC}</author>
-    <author>tc={AFCA1F9F-3656-4D87-B028-158FAC82491A}</author>
     <author>tc={D5F09098-7F1D-4BB7-A6B2-A1BA1A704874}</author>
     <author>tc={CE1E2D36-2C45-4BCE-AE89-C30A66B393BE}</author>
-    <author>tc={1D6C5D70-BF17-4EEC-B30F-90C6BA3581C9}</author>
     <author>tc={94FFD0A4-94E6-44D0-AFF1-E4D74A4A55C2}</author>
     <author>tc={6C1003AE-3D74-420B-93F3-9EB78C864F06}</author>
-    <author>tc={352754FD-B656-49F3-BCAA-2FFE4A505A14}</author>
     <author>tc={59EC36DA-6B9E-413F-89C4-56E9E7E44A89}</author>
-    <author>tc={9D913C7D-0166-4537-882F-9848E15DAC6B}</author>
     <author>tc={24B80C75-97C1-4F68-8BB1-DE33FF04E0FD}</author>
     <author>tc={935001FA-A5BE-4FED-9582-1A6BA84207A5}</author>
-    <author>tc={789F6E67-B991-40BF-9F64-84F8CAAC5041}</author>
     <author>tc={68906487-86CE-4423-968E-A85B0B386C25}</author>
     <author>tc={36725141-628E-4476-A329-125F5473B26F}</author>
-    <author>tc={720155DB-43E9-4E3D-B067-80E33979909F}</author>
     <author>tc={6EF05AFF-6624-4C00-B17D-CDF5A0D6B9A2}</author>
     <author>tc={BB6FCFEC-05A0-43EC-9122-0C14DAE7A149}</author>
-    <author>tc={BA304E9A-5542-409A-B97D-1C87720091F2}</author>
     <author>tc={81C63929-92E1-4141-AC89-6265FEF8F817}</author>
     <author>tc={C592D865-BAF0-40E5-B06F-95DD894CCD3E}</author>
-    <author>tc={161293C4-3808-44F5-87D0-3A58D1DCE9F9}</author>
     <author>tc={9CBE22E1-DFBF-48CA-BB5A-4DF7E0890029}</author>
     <author>tc={0E1ABA66-3073-40B5-A07B-B302C405B9DC}</author>
-    <author>tc={13691A62-9845-4A10-BED2-EA476C092F84}</author>
     <author>tc={4C4EB5D3-295C-4C4C-BCEB-F7E54CBF6B44}</author>
-    <author>tc={D7DFEC19-E955-4AFD-9AAC-0E883202371E}</author>
     <author>tc={6A84BEE9-C34F-407C-A8FF-1723B8A09754}</author>
     <author>tc={CCA9EFE8-A368-486C-A2DF-08D636024BBD}</author>
     <author>tc={2B822552-A796-47C8-AA57-CF3320630FF8}</author>
-    <author>tc={78EB6020-989C-48A3-BE00-A20C1EC63773}</author>
     <author>tc={FA0D8310-A90C-42E4-9210-CD9B57782310}</author>
-    <author>tc={AEA4B76B-7193-4905-A4F4-A5B6D6DD5251}</author>
     <author>tc={E0879D79-098E-41CF-95EB-C39AE1D0159B}</author>
-    <author>tc={D80C5B0D-CFEF-499C-868E-94EAB93E723B}</author>
     <author>tc={A3AE9B5E-0310-4350-9807-69ABC66B6211}</author>
     <author>tc={5D7453CB-76BE-40D2-B145-19184CD3A890}</author>
-    <author>tc={060CC347-F854-423E-9201-C561757B4AD3}</author>
     <author>tc={4726F164-972F-4AA8-9C1B-1471585CA560}</author>
-    <author>tc={695704F7-9606-4A5A-A932-B8C892921EF8}</author>
     <author>tc={B7BA39CD-9FF1-46C7-A57F-300A0D0CA61F}</author>
-    <author>tc={B73FA1FF-4A86-442A-8939-1EB1B3637BC1}</author>
     <author>tc={61AF9F9A-52A3-4A72-A307-527A48F4FF97}</author>
-    <author>tc={B9EF0E84-E789-47B4-A769-C8B7107137C0}</author>
     <author>tc={6A948CD1-63AD-457F-B394-1F7D35C4BE64}</author>
-    <author>tc={F8A8E0E6-D628-47A5-9AFE-D12B9730A1D9}</author>
     <author>tc={94313AA5-1D90-4305-ADF6-5B3D3434DDD2}</author>
     <author>tc={213AD9E0-614E-49A3-845F-60CC7100A896}</author>
-    <author>tc={D4BC4FCD-085E-4655-8B56-3618CE8762AC}</author>
     <author>tc={94BAB893-D779-406F-A7BF-1CBAB6D2086A}</author>
     <author>tc={5CC5811D-5B2C-4D74-9375-385F3E57C90F}</author>
     <author>tc={F5D38346-00B8-44DC-A9FB-E20A879BFC47}</author>
-    <author>tc={9635D360-44C4-400F-AB1B-E928C740858A}</author>
     <author>tc={BFEC1F1B-CA00-429F-8345-09F20773C97F}</author>
     <author>tc={AF894AD0-2B7C-4F99-AF92-5E897151E766}</author>
     <author>tc={3C47F7B2-6A4C-4345-BEDF-BA23749DD7E7}</author>
-    <author>tc={B4BE21C7-4D8E-4A10-A05B-7CB29AFCBF11}</author>
     <author>tc={13AD156E-2609-4291-B347-0A9DC3C370C8}</author>
     <author>tc={D9742BB9-E5BD-4DAC-B08A-8F33A1742026}</author>
-    <author>tc={ECF69508-3E8A-46CC-B588-2FF061AEF2BF}</author>
     <author>tc={2562E7CA-2915-4392-BEB9-1DA6A565E8F7}</author>
     <author>tc={A507645B-D320-4278-AE7D-377365817F29}</author>
-    <author>tc={E240F6D2-DFB8-41B2-967E-7D29D82425D8}</author>
     <author>tc={4ED4155D-4BE2-4D08-A20A-46CCE4600A2F}</author>
     <author>tc={6E3DB2AC-3774-4582-BCA9-9EFF9F0AAE32}</author>
-    <author>tc={D699B47C-3EDF-439F-9760-748B850EC1F9}</author>
     <author>tc={F15400DE-CFAB-4BA5-8732-2025202D8869}</author>
-    <author>tc={FE8BF673-069F-4CC0-85A9-4C68BB190BBB}</author>
     <author>tc={FD7F66CA-0ECB-4CE6-B332-6D2FE5F3C81D}</author>
     <author>tc={0803AB7E-3746-45D3-A8EA-BDFB8B5C1159}</author>
-    <author>tc={41424B6F-041D-4E27-8FE0-4FC215D55379}</author>
     <author>tc={67623983-4763-4197-A23B-53AA436F8A34}</author>
     <author>tc={EB120FF1-5CDA-4D84-A025-CD98307C97C3}</author>
     <author>tc={17A37659-8A9C-4B5F-A3EC-709DD0BCE247}</author>
-    <author>tc={A926AA69-30D0-40C8-AD64-9B94E4C5EF42}</author>
     <author>tc={C2DB1F30-CE98-4E5D-B0C8-B30775816764}</author>
     <author>tc={15242C72-9C7B-495E-B344-131633C4BE80}</author>
     <author>tc={240D5873-44B0-458F-875A-E4225FD1ACAD}</author>
-    <author>tc={B47F104A-FA31-425B-AF50-1422E6F339A4}</author>
     <author>tc={DE897266-EE4C-430B-8A06-36671EA1ECF3}</author>
-    <author>tc={CE50D758-78EF-47CB-8DEF-6F69EB386D92}</author>
     <author>tc={D9DCD7D3-EAA6-44D2-9A62-38FD88896CA6}</author>
-    <author>tc={057CF385-84BB-476C-8E6A-3FB469600EB4}</author>
     <author>tc={CF92684F-E55A-4187-96EE-68B56028E8CB}</author>
-    <author>tc={D3ECDD38-55DB-42AB-8E24-820D4D27690A}</author>
     <author>tc={9626EEC2-270C-466A-BD46-FE28335E7E02}</author>
-    <author>tc={B275DA7B-24DD-46C5-BFD9-1B44FB5FAD46}</author>
     <author>tc={60702B3D-0D4B-4988-B5E8-6A4A2C81D30B}</author>
     <author>tc={6F99AFD3-CF32-4152-A912-1D04F8967B37}</author>
-    <author>tc={AFF19133-139A-4414-B5BD-D26EEAE944C9}</author>
     <author>tc={7DC36BDD-540A-4B1E-9888-76142C106F90}</author>
-    <author>tc={971985CC-EE2C-4CAC-B5F2-03489CB55C67}</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{7F5710BC-5B55-4CAE-8B89-547AD4B6D83A}">
@@ -235,12 +175,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="2" shapeId="0" xr:uid="{E21B303B-A7CD-43D0-B7EA-D905F032D9A5}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner sets out the commission. They work with the analyst team to ensure that everyone has a common understanding of the problem. </t>
+    <comment ref="E3" authorId="2" shapeId="0" xr:uid="{34784133-6C38-415B-9DBC-25B4BCFCC013}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner sets out the commission. They work with the analyst team to ensure that everyone has a common understanding of the problem.</t>
+        </r>
       </text>
     </comment>
     <comment ref="L3" authorId="3" shapeId="0" xr:uid="{B717D9AE-0604-44A0-8412-B2D09E13C4CC}">
@@ -282,24 +227,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="6" shapeId="0" xr:uid="{493BD2CC-B01C-4431-A4D3-5FF34D608502}">
+    <comment ref="E4" authorId="2" shapeId="0" xr:uid="{F1FCD91C-7980-4797-A175-B34F925647D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst must document the purpose of the analysis and the levels of quality and certainty that are needed to meet user requirements. The commissioner and assurer make sure the analysis aligns with the stated purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="6" shapeId="0" xr:uid="{9CF26141-1975-4AF9-A051-D7457E18733E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analyst must document the purpose of the analysis and the levels of quality and certainty that are needed to meet user requirements. The commissioner and analytical assurer make sure the analysis aligns with the stated purpose.
-</t>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="7" shapeId="0" xr:uid="{9CF26141-1975-4AF9-A051-D7457E18733E}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     What is the need for this analysis or statistical release? </t>
       </text>
     </comment>
-    <comment ref="C5" authorId="8" shapeId="0" xr:uid="{ECE1C9BD-0F1F-48B0-8E29-32AEC4DC9500}">
+    <comment ref="C5" authorId="7" shapeId="0" xr:uid="{ECE1C9BD-0F1F-48B0-8E29-32AEC4DC9500}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -322,23 +271,64 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="9" shapeId="0" xr:uid="{87ABBA1D-1BFB-4597-950F-7EA7A2EF80B2}">
+    <comment ref="E5" authorId="2" shapeId="0" xr:uid="{CF2CEA5C-7CC7-4E99-B295-59AB8A12C13A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that key aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated. They also make sure there is proportionate governance in place to support the analysis and its role in the wider project or programme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="8" shapeId="0" xr:uid="{FDBC8216-3E37-4E41-BCE3-4BA3377DA5C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The commissioner makes sure that key aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated. They also make sure there is proportionate governance in place to support the analysis and its role in the wider project or programme</t>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="10" shapeId="0" xr:uid="{FDBC8216-3E37-4E41-BCE3-4BA3377DA5C0}">
+    Identifying if the work is business critical determines the assurance needed to ensure it is fit for purpose.</t>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="1" shapeId="0" xr:uid="{504CD6B7-2D50-4B41-B4FE-4489A7C9A84D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Q6.1: Produce statistics to a suitable level of quality that means they meet their intended uses and are not misleading</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="2" shapeId="0" xr:uid="{B5335CAF-E138-45E4-B347-21891082FC31}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Business critical models must be managed appropriately so that the right specialists are responsible for developing, using and assuring them.
+Decision-makers need sufficient assurance from an appropriate level in the organisation that the model is fit for purpose before using it to inform a decision. For business critical analysis and modelling, the commissioner should be satisfied with the seniority of the assurer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="9" shapeId="0" xr:uid="{BCCD1820-2B3B-4FEC-8B83-86DBCC941395}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Identifying if the work is business critical determines the assurance needed to ensure it is fit for purpose.</t>
-      </text>
-    </comment>
-    <comment ref="D6" authorId="1" shapeId="0" xr:uid="{504CD6B7-2D50-4B41-B4FE-4489A7C9A84D}">
+    Knowing what your outputs will be used for can ensure they meet user needs. A good understanding of uses is essential for making sure that your analysis is fit for purpose.</t>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{C416C419-641C-4B83-A9F8-B8D8AC79497F}">
       <text>
         <r>
           <rPr>
@@ -348,59 +338,32 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Q6.1: Produce statistics to a suitable level of quality that means they meet their intended uses and are not misleading</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="11" shapeId="0" xr:uid="{8EB3435E-2AD8-4AF9-9477-10355940958D}">
+          <t>V8.2: Actively engage key users of your statistics, such as those in academia, business, civil society, the media and public bodies, to identify the most important questions the statistics need to answer. Report on the findings and your decisions in your annual statistical work programme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="2" shapeId="0" xr:uid="{8A5AA2E7-22E5-420D-98BA-92415B8B57E2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that the right stakeholders have been identified so that the scope and boundaries of the analysis can be appropriately explored. The analyst team and  assurer should also contribute.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L7" authorId="10" shapeId="0" xr:uid="{BC3B8A1E-E152-4A66-BD49-D05803E09CA5}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Business critical models must be managed appropriately so that the right specialists are responsible for developing, using and assuring them.
-Decision-makers need sufficient assurance from an appropriate level in the organisation that the model is fit for purpose before using it to inform a decision. For business critical analysis and modelling, the commissioner should be satisfied with the seniority of the analytical assurer. </t>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="12" shapeId="0" xr:uid="{BCCD1820-2B3B-4FEC-8B83-86DBCC941395}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Knowing what your outputs will be used for can ensure they meet user needs. A good understanding of uses is essential for making sure that your analysis is fit for purpose.</t>
-      </text>
-    </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{C416C419-641C-4B83-A9F8-B8D8AC79497F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>V8.2: Actively engage key users of your statistics, such as those in academia, business, civil society, the media and public bodies, to identify the most important questions the statistics need to answer. Report on the findings and your decisions in your annual statistical work programme</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="13" shapeId="0" xr:uid="{18A1EB84-066B-483A-A278-351D641106BE}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner makes sure that the right stakeholders have been identified so that the scope and boundaries of the analysis can be appropriately explored. The analyst team and analytical assurer should also contribute.
-</t>
-      </text>
-    </comment>
-    <comment ref="L7" authorId="14" shapeId="0" xr:uid="{BC3B8A1E-E152-4A66-BD49-D05803E09CA5}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     Who uses your analysis or statistical release?  </t>
       </text>
     </comment>
-    <comment ref="C8" authorId="15" shapeId="0" xr:uid="{FB0F022A-E355-466D-8B31-2880B5FA0755}">
+    <comment ref="C8" authorId="11" shapeId="0" xr:uid="{FB0F022A-E355-466D-8B31-2880B5FA0755}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -425,16 +388,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="16" shapeId="0" xr:uid="{AA6BAEC1-9530-43AE-A233-E2E7C0374046}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Analysts should explore the analysis requirements and scope with all relevant stakeholders to make sure a wide range of perspectives are sought. The commissioner should be aware and briefed.
-</t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="17" shapeId="0" xr:uid="{FB4107FF-85E4-4674-9C4E-7753AB019F16}">
+    <comment ref="E8" authorId="2" shapeId="0" xr:uid="{609FF600-3D2D-4F9E-B2A8-F3A4BD5B818B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analysts should explore the analysis requirements and scope with all relevant stakeholders to make sure a wide range of perspectives are sought. The commissioner should be aware and briefed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="12" shapeId="0" xr:uid="{FB4107FF-85E4-4674-9C4E-7753AB019F16}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -457,15 +424,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="18" shapeId="0" xr:uid="{EF364E4F-6B64-4BFB-8A60-041DE12319C2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During the design and conduct of analysis, the commissioner should set out details like the level of precision, accuracy and uncertainty that are needed.</t>
-      </text>
-    </comment>
-    <comment ref="L9" authorId="19" shapeId="0" xr:uid="{4D792EE8-5DFC-473C-9F60-5F342A95B67E}">
+    <comment ref="E9" authorId="2" shapeId="0" xr:uid="{153CC857-86A8-43FD-B525-461FC1B8A318}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During the design and conduct of analysis, the commissioner should set out details like the level of precision, accuracy and uncertainty that are needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="13" shapeId="0" xr:uid="{4D792EE8-5DFC-473C-9F60-5F342A95B67E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -473,7 +445,7 @@
     How do you know that your analysis or statistical process is working correctly? </t>
       </text>
     </comment>
-    <comment ref="C10" authorId="20" shapeId="0" xr:uid="{8FABEAEF-BAE0-4A77-A3E0-5BF27B3BD2A3}">
+    <comment ref="C10" authorId="14" shapeId="0" xr:uid="{8FABEAEF-BAE0-4A77-A3E0-5BF27B3BD2A3}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -498,16 +470,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="21" shapeId="0" xr:uid="{4A376BBA-7716-405F-A998-FBDCCFB6D36A}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During commissioning and scoping, the commissioner and analyst will need to make trade-offs between time, resources and quality. They should work together to agree and document the right balance across these constraints.
-</t>
-      </text>
-    </comment>
-    <comment ref="M10" authorId="22" shapeId="0" xr:uid="{297D13ED-C651-43E5-A296-C92BDF8140A0}">
+    <comment ref="E10" authorId="2" shapeId="0" xr:uid="{A569523E-0AB8-44BF-B99D-D8B323B596C1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During commissioning and scoping, the commissioner and analyst will need to make trade-offs between time, resources and quality. They should work together to agree and document the right balance across these constraints.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="15" shapeId="0" xr:uid="{297D13ED-C651-43E5-A296-C92BDF8140A0}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -516,7 +492,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C11" authorId="23" shapeId="0" xr:uid="{B8611E4F-62CB-4E5B-B541-B7D57EDFE31B}">
+    <comment ref="C11" authorId="16" shapeId="0" xr:uid="{B8611E4F-62CB-4E5B-B541-B7D57EDFE31B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -538,15 +514,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="24" shapeId="0" xr:uid="{91DA7871-3F83-489C-9B2C-D097153E5C8B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner makes sure that there is sufficient time and resource for the required level of assurance to be delivered and that they understand the risks when time and resource pressures are unavoidable.</t>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="25" shapeId="0" xr:uid="{DDA67DCB-8363-4F2A-8E2F-D7FD31758CC8}">
+    <comment ref="E11" authorId="2" shapeId="0" xr:uid="{892E5D42-AB64-438F-B359-196595A0435E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that there is sufficient time and resource for the required level of assurance to be delivered and that they understand the risks when time and resource pressures are unavoidable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="17" shapeId="0" xr:uid="{DDA67DCB-8363-4F2A-8E2F-D7FD31758CC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -569,19 +550,24 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="26" shapeId="0" xr:uid="{0229EB7C-8A73-4B9E-9D13-796DEAA70543}">
+    <comment ref="E12" authorId="2" shapeId="0" xr:uid="{E3B2EADD-C2B1-4699-86F2-A7B91A2FD417}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure the analyst team understands the context for the analysis question. This helps the analyst to understand and assess likely risks and determine the right analytical and quality assurance response.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="18" shapeId="0" xr:uid="{4EFF044A-661A-45F8-9173-7EAF843C1921}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The commissioner makes sure the analyst team understands the context for the analysis question. This helps the analyst to understand and assess likely risks and determine the right analytical and quality assurance response.</t>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="27" shapeId="0" xr:uid="{4EFF044A-661A-45F8-9173-7EAF843C1921}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     Clear accountability makes sure that important decisions are signed off by the right people. There should be a clear understanding of who is responsible for managing, producing and quality assuring the analysis in the team.</t>
       </text>
     </comment>
@@ -599,15 +585,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="28" shapeId="0" xr:uid="{0B3233E4-B736-4C2D-AADA-A0925FF322D3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During scoping of the analysis, the commissioner makes sure there is proportionate governance in place to support the analysis and its role in the wider project or programme.</t>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="29" shapeId="0" xr:uid="{B074A2B9-B46E-4830-BCD5-A7D9FC9F80B3}">
+    <comment ref="E13" authorId="2" shapeId="0" xr:uid="{A72DCE57-E0A8-438B-B345-F90BEEA27794}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During scoping of the analysis, the commissioner makes sure there is proportionate governance in place to support the analysis and its role in the wider project or programme.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="19" shapeId="0" xr:uid="{B074A2B9-B46E-4830-BCD5-A7D9FC9F80B3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -630,15 +621,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="30" shapeId="0" xr:uid="{F49D43AA-2830-4C6A-B1BB-5F30B710381C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</t>
-      </text>
-    </comment>
-    <comment ref="M14" authorId="31" shapeId="0" xr:uid="{14C4500A-297B-4DC2-A81E-5404A0E6855E}">
+    <comment ref="E14" authorId="2" shapeId="0" xr:uid="{8638546D-92B9-445B-9AB7-59645EC1A501}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="20" shapeId="0" xr:uid="{14C4500A-297B-4DC2-A81E-5404A0E6855E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -647,7 +643,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C15" authorId="32" shapeId="0" xr:uid="{BDD5D421-F6F7-4018-BBB9-CC062F53505D}">
+    <comment ref="C15" authorId="21" shapeId="0" xr:uid="{BDD5D421-F6F7-4018-BBB9-CC062F53505D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -669,15 +665,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E15" authorId="33" shapeId="0" xr:uid="{A8911257-2BC7-4D42-BB6B-8A505C0946B1}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</t>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="34" shapeId="0" xr:uid="{675351E7-4AAD-4CAE-A63B-A1432693D85A}">
+    <comment ref="E15" authorId="2" shapeId="0" xr:uid="{22C25F25-A312-4AE2-B5A9-7F1CE8C6EAB2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="22" shapeId="0" xr:uid="{675351E7-4AAD-4CAE-A63B-A1432693D85A}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -701,15 +702,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="35" shapeId="0" xr:uid="{16B73972-A012-48B7-A793-DAD887DBB3BF}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analystical assurer should challenge and test the understanding of the problem. The commissioner and analyst work with the analytical assurer to make sure that all share a common understanding.</t>
-      </text>
-    </comment>
-    <comment ref="M16" authorId="36" shapeId="0" xr:uid="{247C10C3-5E6D-4D86-B576-9EA0227FA976}">
+    <comment ref="E16" authorId="2" shapeId="0" xr:uid="{AC174C50-96EE-4777-BA07-72F2FA6B278F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The assurer should challenge and test the understanding of the problem. The commissioner and analyst work with the assurer to make sure that all share a common understanding.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M16" authorId="23" shapeId="0" xr:uid="{247C10C3-5E6D-4D86-B576-9EA0227FA976}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -718,7 +724,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C17" authorId="37" shapeId="0" xr:uid="{8ACF04DB-3056-4F30-B39E-A41DFC39BAD7}">
+    <comment ref="C17" authorId="24" shapeId="0" xr:uid="{8ACF04DB-3056-4F30-B39E-A41DFC39BAD7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -740,16 +746,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="38" shapeId="0" xr:uid="{38227814-F8B1-46EF-ABEB-7DEC64C60144}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.
-If there is a need for urgent action, such as mitigation of unacceptable but uncertain risks, the commissioner may ask for further analysis. They might also commission extra evidence-gathering in parallel to inform the policy response when uncertainty is reduced. The analytical assurer must advise the commissioner on whether sufficient analytical quality assurance has happened and inform them about any outstanding risks. </t>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="39" shapeId="0" xr:uid="{59656D8A-69E5-4CDB-8CA0-48493A72EB6E}">
+    <comment ref="E17" authorId="2" shapeId="0" xr:uid="{FC585505-258E-437B-88AB-5780E32946CC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.
+If there is a need for urgent action, such as mitigation of unacceptable but uncertain risks, the commissioner may ask for further analysis. They might also commission extra evidence-gathering in parallel to inform the policy response when uncertainty is reduced. The assurer must advise the commissioner on whether sufficient analytical quality assurance has happened and inform them about any outstanding risks.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="25" shapeId="0" xr:uid="{59656D8A-69E5-4CDB-8CA0-48493A72EB6E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -771,15 +782,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="40" shapeId="0" xr:uid="{65E6E0EC-BC6A-4935-A14C-FBA6D651D1C0}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should make sure that there is appropriate ethical approval for the analysis. The commissioner and analytical assurer should be informed.</t>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="41" shapeId="0" xr:uid="{6326AB4D-3C57-460D-B340-3271BFEA81A2}">
+    <comment ref="E18" authorId="2" shapeId="0" xr:uid="{36495131-EABC-4545-AB75-026A89E64140}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should make sure that there is appropriate ethical approval for the analysis. The commissioner and assurer should be informed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="26" shapeId="0" xr:uid="{6326AB4D-3C57-460D-B340-3271BFEA81A2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -802,16 +818,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="42" shapeId="0" xr:uid="{E0E21280-EAE1-4A23-948F-48D7D64315E4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner and the analyst work together at the scoping stage to get a clear understanding of analytical requirements. During scoping, the commissioner makes sure that the right aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated.
-</t>
-      </text>
-    </comment>
-    <comment ref="C20" authorId="43" shapeId="0" xr:uid="{C2A9A967-BCAA-453B-9DE1-A1889DA749F8}">
+    <comment ref="E19" authorId="2" shapeId="0" xr:uid="{0BE8DE88-D99A-49F2-AF48-A4FCDD45CFBA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner and the analyst work together at the scoping stage to get a clear understanding of analytical requirements. During scoping, the commissioner makes sure that the right aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="27" shapeId="0" xr:uid="{C2A9A967-BCAA-453B-9DE1-A1889DA749F8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -834,19 +854,24 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="44" shapeId="0" xr:uid="{5BC7BB64-C399-4C88-910A-EE0A196D541B}">
+    <comment ref="E20" authorId="2" shapeId="0" xr:uid="{0337FA0F-86F3-4045-AFD0-AC9FB0104390}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The assurer makes sure quality assurance plans for the analysis are appropriate for the decision it supports. All analysis requires some level of quality assurance. Analyst and commissioner should be involved.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="28" shapeId="0" xr:uid="{71D7AD01-61DA-4F82-B9B6-13FA8081889E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analytical assurer makes sure quality assurance plans for the analysis are appropriate for the decision it supports. All analysis requires some level of quality assurance. Analyst and commissioner should be involved.</t>
-      </text>
-    </comment>
-    <comment ref="C21" authorId="45" shapeId="0" xr:uid="{71D7AD01-61DA-4F82-B9B6-13FA8081889E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     You should commission external specialists to peer review or audit the analysis in proportion to risks around use. They should be able to draw on expertise and experience across government and beyond to get feedback, exchange experience and suggest best practice to improve the analysis.</t>
       </text>
     </comment>
@@ -864,15 +889,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="46" shapeId="0" xr:uid="{94791D6F-A09E-4058-A847-C891B2C626C4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analytical assurer should challenge the proposed approach. Check that it delivers as intended and meets customer needs. It is good practice to engage subject matter experts in this review. Analyst and commissioner should be involved.</t>
-      </text>
-    </comment>
-    <comment ref="M21" authorId="47" shapeId="0" xr:uid="{2711FEBA-50F1-49C4-BBCD-00FD8773322F}">
+    <comment ref="E21" authorId="2" shapeId="0" xr:uid="{E65AE9AC-E18C-40C3-944F-0DCFF378AD9F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The assurer should challenge the proposed approach. Check that it delivers as intended and meets customer needs. It is good practice to engage subject matter experts in this review. Analyst and commissioner should be involved.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M21" authorId="29" shapeId="0" xr:uid="{2711FEBA-50F1-49C4-BBCD-00FD8773322F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -881,7 +911,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C22" authorId="48" shapeId="0" xr:uid="{C9BBB705-34D0-4287-A9AF-3DC9914279E0}">
+    <comment ref="C22" authorId="30" shapeId="0" xr:uid="{C9BBB705-34D0-4287-A9AF-3DC9914279E0}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -904,16 +934,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="49" shapeId="0" xr:uid="{816A930F-38AC-4BF9-B788-9577B0D60F19}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer should give feedback to make sure documentation is fit for purpose.
-</t>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="50" shapeId="0" xr:uid="{1F0E8DDD-3806-4EB2-A559-E138AD955876}">
+    <comment ref="E22" authorId="2" shapeId="0" xr:uid="{F1734255-E7EE-4A66-94B5-1422144D058B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The assurer should give feedback to make sure documentation is fit for purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="31" shapeId="0" xr:uid="{1F0E8DDD-3806-4EB2-A559-E138AD955876}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -936,24 +970,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E23" authorId="51" shapeId="0" xr:uid="{13E8362D-B596-42DC-A9CB-A062A4B94158}">
+    <comment ref="E23" authorId="2" shapeId="0" xr:uid="{15025A27-892D-4D66-92FB-D607B975DEDD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The assurer should give feedback to make sure documentation is fit for purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L23" authorId="32" shapeId="0" xr:uid="{5EB69C75-C40A-4B3C-A1C9-C76AB1F55EF6}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer should give feedback to make sure documentation is fit for purpose.
-</t>
-      </text>
-    </comment>
-    <comment ref="L23" authorId="52" shapeId="0" xr:uid="{5EB69C75-C40A-4B3C-A1C9-C76AB1F55EF6}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     Can you summarise and explain the end-to-end process of your analysis or statistical release for somebody who asks about it? </t>
       </text>
     </comment>
-    <comment ref="M23" authorId="53" shapeId="0" xr:uid="{E96E4235-11DB-49F7-9E37-142BBEE9E7C0}">
+    <comment ref="M23" authorId="33" shapeId="0" xr:uid="{E96E4235-11DB-49F7-9E37-142BBEE9E7C0}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -962,7 +1000,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C24" authorId="54" shapeId="0" xr:uid="{41BE326F-BE7B-4F34-83F1-BA0897CC104B}">
+    <comment ref="C24" authorId="34" shapeId="0" xr:uid="{41BE326F-BE7B-4F34-83F1-BA0897CC104B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -985,16 +1023,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E24" authorId="55" shapeId="0" xr:uid="{278AF0F5-1106-492A-AB60-8B0CBF7DA4D5}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst and commissioner should work together during scoping to set out and agree trade-offs between time, resources and quality and establish the optimal balance of these constraints.
-</t>
-      </text>
-    </comment>
-    <comment ref="M24" authorId="56" shapeId="0" xr:uid="{CF291131-C014-40E1-8BDC-CE14CA286B85}">
+    <comment ref="E24" authorId="2" shapeId="0" xr:uid="{9A66A3D3-BE76-4F3E-828F-1E2A37FDCF27}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst and commissioner should work together during scoping to set out and agree trade-offs between time, resources and quality and establish the optimal balance of these constraints.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M24" authorId="35" shapeId="0" xr:uid="{CF291131-C014-40E1-8BDC-CE14CA286B85}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1003,7 +1045,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C25" authorId="57" shapeId="0" xr:uid="{76246FCF-D76F-44ED-98BE-AD6F708D60CB}">
+    <comment ref="C25" authorId="36" shapeId="0" xr:uid="{76246FCF-D76F-44ED-98BE-AD6F708D60CB}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1027,16 +1069,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="58" shapeId="0" xr:uid="{A8AE3539-0828-48D7-85A6-95E81786F997}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should use a risk-based approach to understand the areas of greatest potential error and focus assurance efforts on these areas. The analyst should brief the commissioner so they understand the impact of any reduction in the thoroughness of analytical quality assurance activities.
-</t>
-      </text>
-    </comment>
-    <comment ref="M25" authorId="59" shapeId="0" xr:uid="{75DDAEFF-7FE9-48F4-B766-4CAA33B2B677}">
+    <comment ref="E25" authorId="2" shapeId="0" xr:uid="{D85E1653-6F0F-4FC7-874E-232EC4ED272C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should use a risk-based approach to understand the areas of greatest potential error and focus assurance efforts on these areas. The analyst should brief the commissioner so they understand the impact of any reduction in the thoroughness of analytical quality assurance activities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M25" authorId="37" shapeId="0" xr:uid="{75DDAEFF-7FE9-48F4-B766-4CAA33B2B677}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1047,7 +1093,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C26" authorId="60" shapeId="0" xr:uid="{0CB30745-6A5E-4281-A26B-58CB004C625C}">
+    <comment ref="C26" authorId="38" shapeId="0" xr:uid="{0CB30745-6A5E-4281-A26B-58CB004C625C}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1071,24 +1117,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="61" shapeId="0" xr:uid="{A42575B9-C972-453B-8A32-9A671BEDE603}">
+    <comment ref="E26" authorId="2" shapeId="0" xr:uid="{260FF63D-4E38-4B9C-A727-D455A9A57C04}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should use a risk-based approach to highlight the areas of greatest potential error and focus assurance efforts on these areas.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L26" authorId="39" shapeId="0" xr:uid="{A312EA72-F9CB-4C05-8E8D-7D66458CCD38}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analyst should use a risk-based approach to highlight the areas of greatest potential error and focus assurance efforts on these areas.
-</t>
-      </text>
-    </comment>
-    <comment ref="L26" authorId="62" shapeId="0" xr:uid="{A312EA72-F9CB-4C05-8E8D-7D66458CCD38}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     If you find a mistake in your analysis, do you have a clear and efficient process for addressing the issue and preventing it from happening again? </t>
       </text>
     </comment>
-    <comment ref="M26" authorId="63" shapeId="0" xr:uid="{C78A230B-40F6-4C27-8D15-D5BF92F125EC}">
+    <comment ref="M26" authorId="40" shapeId="0" xr:uid="{C78A230B-40F6-4C27-8D15-D5BF92F125EC}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1099,7 +1149,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C27" authorId="64" shapeId="0" xr:uid="{394075A5-D7F4-4823-90DE-F6DAF78C70F5}">
+    <comment ref="C27" authorId="41" shapeId="0" xr:uid="{394075A5-D7F4-4823-90DE-F6DAF78C70F5}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1122,24 +1172,29 @@
         </r>
       </text>
     </comment>
-    <comment ref="E27" authorId="65" shapeId="0" xr:uid="{FF90D25A-4F6A-4F0E-A1D7-85C575ABF4CF}">
+    <comment ref="E27" authorId="2" shapeId="0" xr:uid="{94CBFD14-0780-406D-9620-472854155083}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Commissioners should expect and require information about uncertainty from analysts. They should challenge them when it is absent, inadequate or ambiguous.
+Commissioners may have identified sources of uncertainty as part of their wider considerations and should share them with the analyst. If the commissioner can explain in advance the impact on decision-making of different degrees of uncertainty, this can help the analyst to design and carry out the analysis at a proportionate level.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L27" authorId="42" shapeId="0" xr:uid="{8680581D-D8CB-43C2-9441-DEA37E980EB7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Commissioners should expect and require information about uncertainty from analysts. They should challenge them when it is absent, inadequate or ambiguous.
-Commissioners may have identified sources of uncertainty as part of their wider considerations and should share them with the analyst. If the commissioner can explain in advance the impact on decision-making of different degrees of uncertainty, this can help the analyst to design and carry out the analysis at a proportionate level. </t>
-      </text>
-    </comment>
-    <comment ref="L27" authorId="66" shapeId="0" xr:uid="{8680581D-D8CB-43C2-9441-DEA37E980EB7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     How do you measure and report uncertainty in your analysis or statistical release? </t>
       </text>
     </comment>
-    <comment ref="C28" authorId="67" shapeId="0" xr:uid="{D988F73F-692A-43EF-A4EA-3CD1684C9B6D}">
+    <comment ref="C28" authorId="43" shapeId="0" xr:uid="{D988F73F-692A-43EF-A4EA-3CD1684C9B6D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1161,16 +1216,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E28" authorId="68" shapeId="0" xr:uid="{1B01FECE-7BE0-4343-BCCC-DAEB90C40E6F}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should collect and manage the data. They must understand data accuracy and uncertainties and capture, manage and understand assumptions. Analytical assurer should check that data processing is sufficient to ensure fitness for purpose.
-</t>
-      </text>
-    </comment>
-    <comment ref="C29" authorId="69" shapeId="0" xr:uid="{1F976AE5-334F-44B3-8203-575633C5DBA1}">
+    <comment ref="E28" authorId="2" shapeId="0" xr:uid="{B6C2F6E4-3A74-4469-B04F-8D44EDDE34D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should collect and manage the data. They must understand data accuracy and uncertainties and capture, manage and understand assumptions. Assurer should check that data processing is sufficient to ensure fitness for purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="44" shapeId="0" xr:uid="{1F976AE5-334F-44B3-8203-575633C5DBA1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1192,15 +1251,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E29" authorId="70" shapeId="0" xr:uid="{33FFCD26-892E-48CB-9570-5772ACF052DA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The analyst should engage appropriate subject matter experts at the appropriate time. The commissioner may be a subject matter expert. The analytical assurer should check that there is sufficient assurance around the choice of data.</t>
-      </text>
-    </comment>
-    <comment ref="C30" authorId="71" shapeId="0" xr:uid="{AE45F985-AF8D-42E4-9B36-D04CCB025BDC}">
+    <comment ref="E29" authorId="2" shapeId="0" xr:uid="{F2014A1B-5069-4F49-B1AC-06AD3D56A399}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The analyst should engage appropriate subject matter experts at the appropriate time. The commissioner may be a subject matter expert. The assurer should check that there is sufficient assurance around the choice of data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="45" shapeId="0" xr:uid="{AE45F985-AF8D-42E4-9B36-D04CCB025BDC}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1224,15 +1288,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E30" authorId="72" shapeId="0" xr:uid="{AFCA1F9F-3656-4D87-B028-158FAC82491A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. Analytical assurer should make sure there is sufficient consideration of strengths and limitations of data.</t>
-      </text>
-    </comment>
-    <comment ref="L30" authorId="73" shapeId="0" xr:uid="{D5F09098-7F1D-4BB7-A6B2-A1BA1A704874}">
+    <comment ref="E30" authorId="2" shapeId="0" xr:uid="{71E48A79-30B9-4C99-9453-E4210C9384C5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. Assurer should make sure there is sufficient consideration of strengths and limitations of data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L30" authorId="46" shapeId="0" xr:uid="{D5F09098-7F1D-4BB7-A6B2-A1BA1A704874}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1240,7 +1309,7 @@
     What is the quality of the data that you use? </t>
       </text>
     </comment>
-    <comment ref="C31" authorId="74" shapeId="0" xr:uid="{CE1E2D36-2C45-4BCE-AE89-C30A66B393BE}">
+    <comment ref="C31" authorId="47" shapeId="0" xr:uid="{CE1E2D36-2C45-4BCE-AE89-C30A66B393BE}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1263,15 +1332,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E31" authorId="75" shapeId="0" xr:uid="{1D6C5D70-BF17-4EEC-B30F-90C6BA3581C9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analytical assurer should expect to see evidence that there has been sufficient dialogue between analysts and the providers of data and other evidence sources.</t>
-      </text>
-    </comment>
-    <comment ref="M31" authorId="76" shapeId="0" xr:uid="{94FFD0A4-94E6-44D0-AFF1-E4D74A4A55C2}">
+    <comment ref="E31" authorId="2" shapeId="0" xr:uid="{3AC4812F-9E18-4985-896D-07D19165D333}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The assurer should expect to see evidence that there has been sufficient dialogue between analysts and the providers of data and other evidence sources.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M31" authorId="48" shapeId="0" xr:uid="{94FFD0A4-94E6-44D0-AFF1-E4D74A4A55C2}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1281,7 +1355,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C32" authorId="77" shapeId="0" xr:uid="{6C1003AE-3D74-420B-93F3-9EB78C864F06}">
+    <comment ref="C32" authorId="49" shapeId="0" xr:uid="{6C1003AE-3D74-420B-93F3-9EB78C864F06}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1304,15 +1378,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="78" shapeId="0" xr:uid="{352754FD-B656-49F3-BCAA-2FFE4A505A14}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should ensure data formats, units, and context are properly understood and handled. They should design and implement quality checks to validate data inputs as required. Analytical assurer should verify that the right assurance is in place.</t>
-      </text>
-    </comment>
-    <comment ref="C33" authorId="79" shapeId="0" xr:uid="{59EC36DA-6B9E-413F-89C4-56E9E7E44A89}">
+    <comment ref="E32" authorId="2" shapeId="0" xr:uid="{294A26EF-86B4-4A70-AADD-C14E0E15518D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should ensure data formats, units, and context are properly understood and handled. They should design and implement quality checks to validate data inputs as required. Assurer should verify that the right assurance is in place.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="50" shapeId="0" xr:uid="{59EC36DA-6B9E-413F-89C4-56E9E7E44A89}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1335,15 +1414,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="80" shapeId="0" xr:uid="{9D913C7D-0166-4537-882F-9848E15DAC6B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner may need to provide the analyst with agreement to use specific data. The analyst should ensure data formats, units, and context are properly understood and handled. Analytical assurer should verify that assurance is in place.</t>
-      </text>
-    </comment>
-    <comment ref="M33" authorId="81" shapeId="0" xr:uid="{24B80C75-97C1-4F68-8BB1-DE33FF04E0FD}">
+    <comment ref="E33" authorId="2" shapeId="0" xr:uid="{9379F27B-1956-4418-BC4C-6240D224C5CA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner may need to provide the analyst with agreement to use specific data. The analyst should ensure data formats, units, and context are properly understood and handled. Assurer should verify that assurance is in place.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="51" shapeId="0" xr:uid="{24B80C75-97C1-4F68-8BB1-DE33FF04E0FD}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1352,7 +1436,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C34" authorId="82" shapeId="0" xr:uid="{935001FA-A5BE-4FED-9582-1A6BA84207A5}">
+    <comment ref="C34" authorId="52" shapeId="0" xr:uid="{935001FA-A5BE-4FED-9582-1A6BA84207A5}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1375,15 +1459,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="83" shapeId="0" xr:uid="{789F6E67-B991-40BF-9F64-84F8CAAC5041}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The analytical assurer should assess whether assurance is sufficient.</t>
-      </text>
-    </comment>
-    <comment ref="M34" authorId="84" shapeId="0" xr:uid="{68906487-86CE-4423-968E-A85B0B386C25}">
+    <comment ref="E34" authorId="2" shapeId="0" xr:uid="{38F7A734-3C85-425F-A6F4-BD89A0EA6085}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The assurer should assess whether assurance is sufficient.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M34" authorId="53" shapeId="0" xr:uid="{68906487-86CE-4423-968E-A85B0B386C25}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1392,7 +1481,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C35" authorId="85" shapeId="0" xr:uid="{36725141-628E-4476-A329-125F5473B26F}">
+    <comment ref="C35" authorId="54" shapeId="0" xr:uid="{36725141-628E-4476-A329-125F5473B26F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1415,16 +1504,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E35" authorId="86" shapeId="0" xr:uid="{720155DB-43E9-4E3D-B067-80E33979909F}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During the design and conduct of analysis, the commissioner may need to provide the analyst with information, agreement to use resources or confirmation of assumptions or approach. The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The analytical assurer checks that assurance and mitigation are sufficient.
-</t>
-      </text>
-    </comment>
-    <comment ref="M35" authorId="87" shapeId="0" xr:uid="{6EF05AFF-6624-4C00-B17D-CDF5A0D6B9A2}">
+    <comment ref="E35" authorId="2" shapeId="0" xr:uid="{5131D162-FE18-4323-B4B3-3C244C772125}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During the design and conduct of analysis, the commissioner may need to provide the analyst with information, agreement to use resources or confirmation of assumptions or approach. The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The assurer checks that assurance and mitigation are sufficient.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M35" authorId="55" shapeId="0" xr:uid="{6EF05AFF-6624-4C00-B17D-CDF5A0D6B9A2}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1433,7 +1526,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C36" authorId="88" shapeId="0" xr:uid="{BB6FCFEC-05A0-43EC-9122-0C14DAE7A149}">
+    <comment ref="C36" authorId="56" shapeId="0" xr:uid="{BB6FCFEC-05A0-43EC-9122-0C14DAE7A149}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1456,16 +1549,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E36" authorId="89" shapeId="0" xr:uid="{BA304E9A-5542-409A-B97D-1C87720091F2}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During the design and conduct of analysis, the commissioner provides the analyst with the information they need for the analysis to proceed. This could include agreement to use datasets, setting out of key assumptions and signing off assumptions developed during the project. Analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The analytical assurer checks that assurance and mitigation are sufficient.
-</t>
-      </text>
-    </comment>
-    <comment ref="M36" authorId="90" shapeId="0" xr:uid="{81C63929-92E1-4141-AC89-6265FEF8F817}">
+    <comment ref="E36" authorId="2" shapeId="0" xr:uid="{A408E4C6-6EFD-477A-8B8E-23CECBAA2223}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During the design and conduct of analysis, the commissioner provides the analyst with the information they need for the analysis to proceed. This could include agreement to use datasets, setting out of key assumptions and signing off assumptions developed during the project. Analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The assurer checks that assurance and mitigation are sufficient.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M36" authorId="57" shapeId="0" xr:uid="{81C63929-92E1-4141-AC89-6265FEF8F817}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1474,7 +1571,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C37" authorId="91" shapeId="0" xr:uid="{C592D865-BAF0-40E5-B06F-95DD894CCD3E}">
+    <comment ref="C37" authorId="58" shapeId="0" xr:uid="{C592D865-BAF0-40E5-B06F-95DD894CCD3E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1496,15 +1593,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E37" authorId="92" shapeId="0" xr:uid="{161293C4-3808-44F5-87D0-3A58D1DCE9F9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    During the design phase, the analyst will convert the commission into an analytical plan and will consider inputs, analytical methods and processes, and expected outputs. The analytical assurer should check that the proposed design meets the commissioner’s requirements and is sufficiently assured.</t>
-      </text>
-    </comment>
-    <comment ref="L37" authorId="93" shapeId="0" xr:uid="{9CBE22E1-DFBF-48CA-BB5A-4DF7E0890029}">
+    <comment ref="E37" authorId="2" shapeId="0" xr:uid="{91C41846-B9EA-4542-B546-08C37107C949}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During the design phase, the analyst will convert the commission into an analytical plan and will consider inputs, analytical methods and processes, and expected outputs. The assurer should check that the proposed design meets the commissioner’s requirements and is sufficiently assured.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L37" authorId="59" shapeId="0" xr:uid="{9CBE22E1-DFBF-48CA-BB5A-4DF7E0890029}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1514,7 +1616,7 @@
     How do you know the method you are using is appropriate? </t>
       </text>
     </comment>
-    <comment ref="C38" authorId="94" shapeId="0" xr:uid="{0E1ABA66-3073-40B5-A07B-B302C405B9DC}">
+    <comment ref="C38" authorId="60" shapeId="0" xr:uid="{0E1ABA66-3073-40B5-A07B-B302C405B9DC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1536,54 +1638,63 @@
         </r>
       </text>
     </comment>
-    <comment ref="E38" authorId="95" shapeId="0" xr:uid="{13691A62-9845-4A10-BED2-EA476C092F84}">
+    <comment ref="E38" authorId="2" shapeId="0" xr:uid="{78760DA9-2D6A-4785-9CB6-0D9D4FF9AAAF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should review the analysis as a whole and consider carefully whether there are other, better ways in which it could be done. The assurer should check that the investigation of methods was sufficiently thorough and proportionate.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C39" authorId="61" shapeId="0" xr:uid="{4C4EB5D3-295C-4C4C-BCEB-F7E54CBF6B44}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    You need to be sure that your analysis produces the outputs you think it should and the processes run as expected. If you cannot demonstrate that scripts and processes work correctly, you cannot confirm the quality of the results.</t>
+      </text>
+    </comment>
+    <comment ref="D39" authorId="1" shapeId="0" xr:uid="{B5116DF4-7D59-4E58-BDF8-20E033214484}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Q6.10: Verify that the statistics are representative and of suitable quality and monitor relevant quality dimensions for both input data and the statistics, such as completeness and validity, accuracy and reliability, coherence and comparability, and timeliness. Quantify statistical error, including bias, and produce measures of confidence where possible</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="2" shapeId="0" xr:uid="{5154EFFD-B845-4A2C-B947-E9A34422A04A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should validate that the analysis as set up to answer the specification of the commissioner. The assurer checks that assurance and mitigation are sufficient so the analysis is fit for purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L39" authorId="62" shapeId="0" xr:uid="{6A84BEE9-C34F-407C-A8FF-1723B8A09754}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analyst should review the analysis as a whole and consider carefully whether there are other, better ways in which it could be done. The analytical assurer should check that the investigation of methods was sufficiently thorough and proportionate.
-</t>
-      </text>
-    </comment>
-    <comment ref="C39" authorId="96" shapeId="0" xr:uid="{4C4EB5D3-295C-4C4C-BCEB-F7E54CBF6B44}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    You need to be sure that your analysis produces the outputs you think it should and the processes run as expected. If you cannot demonstrate that scripts and processes work correctly, you cannot confirm the quality of the results.</t>
-      </text>
-    </comment>
-    <comment ref="D39" authorId="1" shapeId="0" xr:uid="{B5116DF4-7D59-4E58-BDF8-20E033214484}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Q6.10: Verify that the statistics are representative and of suitable quality and monitor relevant quality dimensions for both input data and the statistics, such as completeness and validity, accuracy and reliability, coherence and comparability, and timeliness. Quantify statistical error, including bias, and produce measures of confidence where possible</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E39" authorId="97" shapeId="0" xr:uid="{D7DFEC19-E955-4AFD-9AAC-0E883202371E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should validate that the analysis as set up to answer the specification of the commissioner. The analytical assurer checks that assurance and mitigation are sufficient so the analysis is fit for purpose.</t>
-      </text>
-    </comment>
-    <comment ref="L39" authorId="98" shapeId="0" xr:uid="{6A84BEE9-C34F-407C-A8FF-1723B8A09754}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     How do you know that your analysis or statistical process is working correctly? </t>
       </text>
     </comment>
-    <comment ref="M39" authorId="99" shapeId="0" xr:uid="{CCA9EFE8-A368-486C-A2DF-08D636024BBD}">
+    <comment ref="M39" authorId="63" shapeId="0" xr:uid="{CCA9EFE8-A368-486C-A2DF-08D636024BBD}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1594,7 +1705,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C40" authorId="100" shapeId="0" xr:uid="{2B822552-A796-47C8-AA57-CF3320630FF8}">
+    <comment ref="C40" authorId="64" shapeId="0" xr:uid="{2B822552-A796-47C8-AA57-CF3320630FF8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1617,16 +1728,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E40" authorId="101" shapeId="0" xr:uid="{78EB6020-989C-48A3-BE00-A20C1EC63773}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst should capture, manage and understand explicit and implicit assumptions made. The analytical assurer should assess whether these are sufficient. The commissioner should be made aware of key assumptions and confirm that they are happy that the assumptions are applied.
-</t>
-      </text>
-    </comment>
-    <comment ref="C41" authorId="102" shapeId="0" xr:uid="{FA0D8310-A90C-42E4-9210-CD9B57782310}">
+    <comment ref="E40" authorId="2" shapeId="0" xr:uid="{A3148CB9-92F1-45FA-AC2D-0C04FA7C927E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should capture, manage and understand explicit and implicit assumptions made. The assurer should assess whether these are sufficient. The commissioner should be made aware of key assumptions and confirm that they are happy that the assumptions are applied.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="65" shapeId="0" xr:uid="{FA0D8310-A90C-42E4-9210-CD9B57782310}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1650,15 +1765,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E41" authorId="103" shapeId="0" xr:uid="{AEA4B76B-7193-4905-A4F4-A5B6D6DD5251}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain assumptions. Analytical assurer should check that validation and assurance of assumptions is sufficient.</t>
-      </text>
-    </comment>
-    <comment ref="C42" authorId="104" shapeId="0" xr:uid="{E0879D79-098E-41CF-95EB-C39AE1D0159B}">
+    <comment ref="E41" authorId="2" shapeId="0" xr:uid="{B6436E41-91F1-48F8-B4C3-D08358725C7D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain assumptions. Assurer should check that validation and assurance of assumptions is sufficient.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C42" authorId="66" shapeId="0" xr:uid="{E0879D79-098E-41CF-95EB-C39AE1D0159B}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1681,24 +1801,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E42" authorId="105" shapeId="0" xr:uid="{D80C5B0D-CFEF-499C-868E-94EAB93E723B}">
+    <comment ref="E42" authorId="2" shapeId="0" xr:uid="{0D493E16-1410-48D3-8111-FCDDAA2E5DA4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analyst should determine and communicate the uncertainty associated with outputs so that the commissioner can make informed decisions. The range of possible outcomes and their relative likelihoods should be described. The assurer checks that measuring and reporting of uncertainty is sufficient to meet the needs of the commissioner.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L42" authorId="67" shapeId="0" xr:uid="{A3AE9B5E-0310-4350-9807-69ABC66B6211}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Analyst should determine and communicate the uncertainty associated with outputs so that the commissioner can make informed decisions. The range of possible outcomes and their relative likelihoods should be described. The analytical assurer checks that measuring and reporting of uncertainty is sufficient to meet the needs of the commissioner.
-</t>
-      </text>
-    </comment>
-    <comment ref="L42" authorId="106" shapeId="0" xr:uid="{A3AE9B5E-0310-4350-9807-69ABC66B6211}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     How do you measure and report uncertainty in your analysis or statistical release? </t>
       </text>
     </comment>
-    <comment ref="C43" authorId="107" shapeId="0" xr:uid="{5D7453CB-76BE-40D2-B145-19184CD3A890}">
+    <comment ref="C43" authorId="68" shapeId="0" xr:uid="{5D7453CB-76BE-40D2-B145-19184CD3A890}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1720,15 +1844,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="108" shapeId="0" xr:uid="{060CC347-F854-423E-9201-C561757B4AD3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If uncertainties are too complex for analysts to quantify, even approximately, the analysts should say so in order that the commissioner can take this into account.</t>
-      </text>
-    </comment>
-    <comment ref="C44" authorId="109" shapeId="0" xr:uid="{4726F164-972F-4AA8-9C1B-1471585CA560}">
+    <comment ref="E43" authorId="2" shapeId="0" xr:uid="{8306D4C6-1899-47B9-975E-7996713CF3B4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If uncertainties are too complex for analysts to quantify, even approximately, the analysts should say so in order that the commissioner can take this into account.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C44" authorId="69" shapeId="0" xr:uid="{4726F164-972F-4AA8-9C1B-1471585CA560}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1751,16 +1880,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E44" authorId="110" shapeId="0" xr:uid="{695704F7-9606-4A5A-A932-B8C892921EF8}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Analyst should make sure that the implications of data dependencies or relationships to other analysis and methods are understood. Analytical assurer should check that dependencies have been properly considered.
-</t>
-      </text>
-    </comment>
-    <comment ref="C45" authorId="111" shapeId="0" xr:uid="{B7BA39CD-9FF1-46C7-A57F-300A0D0CA61F}">
+    <comment ref="E44" authorId="2" shapeId="0" xr:uid="{5F0AF5DC-1152-4C1B-A9E9-D71A790A95A8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analyst should make sure that the implications of data dependencies or relationships to other analysis and methods are understood. Assurer should check that dependencies have been properly considered.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C45" authorId="70" shapeId="0" xr:uid="{B7BA39CD-9FF1-46C7-A57F-300A0D0CA61F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1783,23 +1916,63 @@
         </r>
       </text>
     </comment>
-    <comment ref="E45" authorId="112" shapeId="0" xr:uid="{B73FA1FF-4A86-442A-8939-1EB1B3637BC1}">
+    <comment ref="E45" authorId="2" shapeId="0" xr:uid="{E98D6DA0-DFEC-4213-95E9-444F0862CBDD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analysis should be peer reviewed at an appropriate and proportionate level by a competent person. Commissioner, analyst and assurer should all be involved in each stage of the analytical cycle.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C46" authorId="71" shapeId="0" xr:uid="{61AF9F9A-52A3-4A72-A307-527A48F4FF97}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Analysis should be peer reviewed at an appropriate and proportionate level by a competent person. Commissioner, analyst and analytical assurer should all be involved in each stage of the analytical cycle.</t>
-      </text>
-    </comment>
-    <comment ref="C46" authorId="113" shapeId="0" xr:uid="{61AF9F9A-52A3-4A72-A307-527A48F4FF97}">
+    All analysis involves decisions. A comprehensive record of the decisions made in specifying and conducting the analysis ensures a full audit trail of why decisions were made, who made them and signed them off.</t>
+      </text>
+    </comment>
+    <comment ref="D46" authorId="1" shapeId="0" xr:uid="{398C2120-3E32-4391-BA6A-867A801FB24B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Q6.7: Base methods on national or international good practice, scientific principles or professional consensus. Identify potential bias and address limitations. Use recognised standards, classifications and definitions. Explain reasons for deviations from these standards and any related implications for use</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E46" authorId="2" shapeId="0" xr:uid="{D2E23DB6-6D72-46E4-98A0-BF9939A57810}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The assurer should make sure that a suitable audit trail is in place that clarifies the level of validation, scope, and risks associated with the analysis. Best practice includes the production of validation log books. Analyst should build this audit trail.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C47" authorId="72" shapeId="0" xr:uid="{6A948CD1-63AD-457F-B394-1F7D35C4BE64}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    All analysis involves decisions. A comprehensive record of the decisions made in specifying and conducting the analysis ensures a full audit trail of why decisions were made, who made them and signed them off.</t>
-      </text>
-    </comment>
-    <comment ref="D46" authorId="1" shapeId="0" xr:uid="{398C2120-3E32-4391-BA6A-867A801FB24B}">
+    Good version control ensures a full understanding of when, why, and how changes were made to your analysis process. If it is hard to track changes, it will be hard to retrace steps if there is a problem and means you do not fully understand the process.</t>
+      </text>
+    </comment>
+    <comment ref="D47" authorId="1" shapeId="0" xr:uid="{0AA4F734-F89C-4F26-9B85-B9BE1917109F}">
       <text>
         <r>
           <rPr>
@@ -1809,50 +1982,24 @@
             <family val="2"/>
             <scheme val="minor"/>
           </rPr>
-          <t>Q6.7: Base methods on national or international good practice, scientific principles or professional consensus. Identify potential bias and address limitations. Use recognised standards, classifications and definitions. Explain reasons for deviations from these standards and any related implications for use</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E46" authorId="114" shapeId="0" xr:uid="{B9EF0E84-E789-47B4-A769-C8B7107137C0}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analytical assurer should make sure that a suitable audit trail is in place that clarifies the level of validation, scope, and risks associated with the analysis. Best practice includes the production of validation log books. Analyst should build this audit trail.</t>
-      </text>
-    </comment>
-    <comment ref="C47" authorId="115" shapeId="0" xr:uid="{6A948CD1-63AD-457F-B394-1F7D35C4BE64}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Good version control ensures a full understanding of when, why, and how changes were made to your analysis process. If it is hard to track changes, it will be hard to retrace steps if there is a problem and means you do not fully understand the process.</t>
-      </text>
-    </comment>
-    <comment ref="D47" authorId="1" shapeId="0" xr:uid="{0AA4F734-F89C-4F26-9B85-B9BE1917109F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
           <t>V10.5: Support the reuse of data and statistics, preventing barriers to use where possible. Ensure statistics are reproducible. Support data and statistics to be shared, accessed and linked, using common data standards with associated metadata</t>
         </r>
       </text>
     </comment>
-    <comment ref="E47" authorId="116" shapeId="0" xr:uid="{F8A8E0E6-D628-47A5-9AFE-D12B9730A1D9}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    To make analytical audit easy, you should set up a version control system for the analysis as a whole and for code, supporting data and assumptions. Best practice includes the production of validation log books. Analyst should build this audit trail. The Analytical assurer should ensure that the audit trail clarifies the level of validation, scope, and risks associated with the analysis.
-</t>
-      </text>
-    </comment>
-    <comment ref="M47" authorId="117" shapeId="0" xr:uid="{94313AA5-1D90-4305-ADF6-5B3D3434DDD2}">
+    <comment ref="E47" authorId="2" shapeId="0" xr:uid="{3F88A162-BBC1-49EB-A470-52366D1F8D2D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>To make analytical audit easy, you should set up a version control system for the analysis as a whole and for code, supporting data and assumptions. Best practice includes the production of validation log books. Analyst should build this audit trail. The assurer should ensure that the audit trail clarifies the level of validation, scope, and risks associated with the analysis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M47" authorId="73" shapeId="0" xr:uid="{94313AA5-1D90-4305-ADF6-5B3D3434DDD2}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1861,7 +2008,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C48" authorId="118" shapeId="0" xr:uid="{213AD9E0-614E-49A3-845F-60CC7100A896}">
+    <comment ref="C48" authorId="74" shapeId="0" xr:uid="{213AD9E0-614E-49A3-845F-60CC7100A896}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1883,15 +2030,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E48" authorId="119" shapeId="0" xr:uid="{D4BC4FCD-085E-4655-8B56-3618CE8762AC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Good quality analysis is reproducible. Analyst should check that the analytical process reflects the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust)</t>
-      </text>
-    </comment>
-    <comment ref="L48" authorId="120" shapeId="0" xr:uid="{94BAB893-D779-406F-A7BF-1CBAB6D2086A}">
+    <comment ref="E48" authorId="2" shapeId="0" xr:uid="{BDCAFEA3-CE54-4728-B99C-F9C2E3CCE128}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Good quality analysis is reproducible. Analyst should check that the analytical process reflects the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L48" authorId="75" shapeId="0" xr:uid="{94BAB893-D779-406F-A7BF-1CBAB6D2086A}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1899,7 +2051,7 @@
     Would another analyst be able to pick up from where you left off and reproduce or continue the work (without talking to you first)? </t>
       </text>
     </comment>
-    <comment ref="M48" authorId="121" shapeId="0" xr:uid="{5CC5811D-5B2C-4D74-9375-385F3E57C90F}">
+    <comment ref="M48" authorId="76" shapeId="0" xr:uid="{5CC5811D-5B2C-4D74-9375-385F3E57C90F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1908,7 +2060,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C49" authorId="122" shapeId="0" xr:uid="{F5D38346-00B8-44DC-A9FB-E20A879BFC47}">
+    <comment ref="C49" authorId="77" shapeId="0" xr:uid="{F5D38346-00B8-44DC-A9FB-E20A879BFC47}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1932,24 +2084,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E49" authorId="123" shapeId="0" xr:uid="{9635D360-44C4-400F-AB1B-E928C740858A}">
+    <comment ref="E49" authorId="2" shapeId="0" xr:uid="{3F06FBB6-EE94-41E4-B87C-55528DBE818E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst should provide proportionate documentation that explains the verification and validation activities that the analysis is subjected to. Analysts must perform appropriate test to check the analysis. They should commission other verification and validation as required. Assurer should confirm that planned validation and verification are sufficient.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L49" authorId="78" shapeId="0" xr:uid="{BFEC1F1B-CA00-429F-8345-09F20773C97F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The analyst should provide proportionate documentation that explains the verification and validation activities that the analysis is subjected to. Analysts must perform appropriate test to check the analysis. They should commission other verification and validation as required. Analytical assurer should confirm that planned validation and verification are sufficient.
-</t>
-      </text>
-    </comment>
-    <comment ref="L49" authorId="124" shapeId="0" xr:uid="{BFEC1F1B-CA00-429F-8345-09F20773C97F}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     Do you consistently use peer review to check scripts and code, documentation, implementation of methods, processes and outputs? </t>
       </text>
     </comment>
-    <comment ref="M49" authorId="125" shapeId="0" xr:uid="{AF894AD0-2B7C-4F99-AF92-5E897151E766}">
+    <comment ref="M49" authorId="79" shapeId="0" xr:uid="{AF894AD0-2B7C-4F99-AF92-5E897151E766}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1960,7 +2116,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C50" authorId="126" shapeId="0" xr:uid="{3C47F7B2-6A4C-4345-BEDF-BA23749DD7E7}">
+    <comment ref="C50" authorId="80" shapeId="0" xr:uid="{3C47F7B2-6A4C-4345-BEDF-BA23749DD7E7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1983,16 +2139,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E50" authorId="127" shapeId="0" xr:uid="{B4BE21C7-4D8E-4A10-A05B-7CB29AFCBF11}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Analysts should work with the commissioner to set out the analysis question so that appropriate analysis is done. Some analysis may require external specialists, so analysts may have responsibilities as part of the procurement process. Analysts, including 3rd parties providing analysis, should provide proportionate documentation describing the verification and validation activities undertaken and associated conclusions. The analytical assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.
-</t>
-      </text>
-    </comment>
-    <comment ref="M50" authorId="128" shapeId="0" xr:uid="{13AD156E-2609-4291-B347-0A9DC3C370C8}">
+    <comment ref="E50" authorId="2" shapeId="0" xr:uid="{C260BF4C-C3E9-4160-9847-31B6466EAF97}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analysts should work with the commissioner to set out the analysis question so that appropriate analysis is done. Some analysis may require external specialists, so analysts may have responsibilities as part of the procurement process. Analysts, including 3rd parties providing analysis, should provide proportionate documentation describing the verification and validation activities undertaken and associated conclusions. The assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M50" authorId="81" shapeId="0" xr:uid="{13AD156E-2609-4291-B347-0A9DC3C370C8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2001,7 +2161,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C51" authorId="129" shapeId="0" xr:uid="{D9742BB9-E5BD-4DAC-B08A-8F33A1742026}">
+    <comment ref="C51" authorId="82" shapeId="0" xr:uid="{D9742BB9-E5BD-4DAC-B08A-8F33A1742026}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2025,24 +2185,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E51" authorId="130" shapeId="0" xr:uid="{ECF69508-3E8A-46CC-B588-2FF061AEF2BF}">
+    <comment ref="E51" authorId="2" shapeId="0" xr:uid="{D5F4F55F-3BFA-4844-B7D5-95ED2864164F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>As part of the delivery phase, the commissioner should ensure there is an assessment of the level of analytical quality assurance of the analysis, noting where there have been trade-offs between time, resources and quality. The assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L51" authorId="83" shapeId="0" xr:uid="{2562E7CA-2915-4392-BEB9-1DA6A565E8F7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    As part of the delivery phase, the commissioner should ensure there is an assessment of the level of analytical quality assurance of the analysis, noting where there have been trade-offs between time, resources and quality. The analytical assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.
-</t>
-      </text>
-    </comment>
-    <comment ref="L51" authorId="131" shapeId="0" xr:uid="{2562E7CA-2915-4392-BEB9-1DA6A565E8F7}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     What is the assessment of the quality of your analytical outputs? </t>
       </text>
     </comment>
-    <comment ref="C52" authorId="132" shapeId="0" xr:uid="{A507645B-D320-4278-AE7D-377365817F29}">
+    <comment ref="C52" authorId="84" shapeId="0" xr:uid="{A507645B-D320-4278-AE7D-377365817F29}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2066,15 +2230,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E52" authorId="133" shapeId="0" xr:uid="{E240F6D2-DFB8-41B2-967E-7D29D82425D8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst must build in checks and processes to ensure that the analysis is correct. During the delivery phase, the commissioner should give feedback to assist in the correct interpretation of results and determine if the analysis has addressed the commission. The analyst should work with the analytical assurer while doing the analysis so that they can comment on whether the analysis meets the needs of the commission to ensure best use of the results</t>
-      </text>
-    </comment>
-    <comment ref="M52" authorId="134" shapeId="0" xr:uid="{4ED4155D-4BE2-4D08-A20A-46CCE4600A2F}">
+    <comment ref="E52" authorId="2" shapeId="0" xr:uid="{EEC565DA-B2BF-43E5-87F8-CAB6B9693351}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst must build in checks and processes to ensure that the analysis is correct. During the delivery phase, the commissioner should give feedback to assist in the correct interpretation of results and determine if the analysis has addressed the commission. The analyst should work with the analytical assurer while doing the analysis so that they can comment on whether the analysis meets the needs of the commission to ensure best use of the results</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M52" authorId="85" shapeId="0" xr:uid="{4ED4155D-4BE2-4D08-A20A-46CCE4600A2F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2085,7 +2254,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C53" authorId="135" shapeId="0" xr:uid="{6E3DB2AC-3774-4582-BCA9-9EFF9F0AAE32}">
+    <comment ref="C53" authorId="86" shapeId="0" xr:uid="{6E3DB2AC-3774-4582-BCA9-9EFF9F0AAE32}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2107,15 +2276,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E53" authorId="136" shapeId="0" xr:uid="{D699B47C-3EDF-439F-9760-748B850EC1F9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    When interpreting the results of a piece of analysis, the commissioner provides constructive challenge. They work with the analyst to explore whether further analysis is needed.</t>
-      </text>
-    </comment>
-    <comment ref="C54" authorId="137" shapeId="0" xr:uid="{F15400DE-CFAB-4BA5-8732-2025202D8869}">
+    <comment ref="E53" authorId="2" shapeId="0" xr:uid="{A2CB388C-08F6-405A-B26A-37477B6B54AE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>When interpreting the results of a piece of analysis, the commissioner provides constructive challenge. They work with the analyst to explore whether further analysis is needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C54" authorId="87" shapeId="0" xr:uid="{F15400DE-CFAB-4BA5-8732-2025202D8869}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2139,15 +2313,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E54" authorId="138" shapeId="0" xr:uid="{FE8BF673-069F-4CC0-85A9-4C68BB190BBB}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. The analysis plan should include treatment of unusual values and outliers. Analytical assurer should be involved.</t>
-      </text>
-    </comment>
-    <comment ref="M54" authorId="139" shapeId="0" xr:uid="{FD7F66CA-0ECB-4CE6-B332-6D2FE5F3C81D}">
+    <comment ref="E54" authorId="2" shapeId="0" xr:uid="{C7CAEAEE-FA7D-46E2-8749-AB902063EF57}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. The analysis plan should include treatment of unusual values and outliers. Assurer should be involved.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M54" authorId="88" shapeId="0" xr:uid="{FD7F66CA-0ECB-4CE6-B332-6D2FE5F3C81D}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2156,7 +2335,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C55" authorId="140" shapeId="0" xr:uid="{0803AB7E-3746-45D3-A8EA-BDFB8B5C1159}">
+    <comment ref="C55" authorId="89" shapeId="0" xr:uid="{0803AB7E-3746-45D3-A8EA-BDFB8B5C1159}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2178,24 +2357,28 @@
         </r>
       </text>
     </comment>
-    <comment ref="E55" authorId="141" shapeId="0" xr:uid="{41424B6F-041D-4E27-8FE0-4FC215D55379}">
+    <comment ref="E55" authorId="2" shapeId="0" xr:uid="{93971D48-5531-4516-8E05-1E48DF9E36B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>During the delivery phase, the commissioner receives the results of the analysis and decides whether it meets their needs. The analyst provides sufficient information to support the commissioner to make an informed decision.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L55" authorId="90" shapeId="0" xr:uid="{67623983-4763-4197-A23B-53AA436F8A34}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    During the delivery phase, the commissioner receives the results of the analysis and decides whether it meets their needs. The analyst provides sufficient information to support the commissioner to make an informed decision.
-</t>
-      </text>
-    </comment>
-    <comment ref="L55" authorId="142" shapeId="0" xr:uid="{67623983-4763-4197-A23B-53AA436F8A34}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
     Could you give a clear account of what can and cannot be inferred from your analysis or statistical release? </t>
       </text>
     </comment>
-    <comment ref="M55" authorId="143" shapeId="0" xr:uid="{EB120FF1-5CDA-4D84-A025-CD98307C97C3}">
+    <comment ref="M55" authorId="91" shapeId="0" xr:uid="{EB120FF1-5CDA-4D84-A025-CD98307C97C3}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2204,7 +2387,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C56" authorId="144" shapeId="0" xr:uid="{17A37659-8A9C-4B5F-A3EC-709DD0BCE247}">
+    <comment ref="C56" authorId="92" shapeId="0" xr:uid="{17A37659-8A9C-4B5F-A3EC-709DD0BCE247}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2228,16 +2411,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E56" authorId="145" shapeId="0" xr:uid="{A926AA69-30D0-40C8-AD64-9B94E4C5EF42}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The commissioner must be confident in the quality of the outputs. They should understand the strengths, limitations and context of the analysis so that the results are correctly interpreted. Analytical assurer sign-off provides confidence that analysis risks, limitations and major assumptions are understood by the users of the analysis. Analysts make sure that the commissioner and analytical assurer have the evidence they need.
-</t>
-      </text>
-    </comment>
-    <comment ref="L56" authorId="146" shapeId="0" xr:uid="{C2DB1F30-CE98-4E5D-B0C8-B30775816764}">
+    <comment ref="E56" authorId="2" shapeId="0" xr:uid="{A2D8C03F-A6F3-439E-BD86-0930022EEA30}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The commissioner must be confident in the quality of the outputs. They should understand the strengths, limitations and context of the analysis so that the results are correctly interpreted. Analytical assurer sign-off provides confidence that analysis risks, limitations and major assumptions are understood by the users of the analysis. Analysts make sure that the commissioner and assurer have the evidence they need.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L56" authorId="93" shapeId="0" xr:uid="{C2DB1F30-CE98-4E5D-B0C8-B30775816764}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2247,7 +2434,7 @@
     Have you assessed the impact of the limitations and set out how they will affect the quality and use of the outputs? </t>
       </text>
     </comment>
-    <comment ref="M56" authorId="147" shapeId="0" xr:uid="{15242C72-9C7B-495E-B344-131633C4BE80}">
+    <comment ref="M56" authorId="94" shapeId="0" xr:uid="{15242C72-9C7B-495E-B344-131633C4BE80}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2256,7 +2443,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C57" authorId="148" shapeId="0" xr:uid="{240D5873-44B0-458F-875A-E4225FD1ACAD}">
+    <comment ref="C57" authorId="95" shapeId="0" xr:uid="{240D5873-44B0-458F-875A-E4225FD1ACAD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2278,15 +2465,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E57" authorId="149" shapeId="0" xr:uid="{B47F104A-FA31-425B-AF50-1422E6F339A4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst and analytical assurer should enable and encourage peer review. Peer reviews provide useful critical challenge about the analytical approach, application of methods and interpretation of the analysis. Verification and peer review of work should be done by analysts who had no involvement in the work so their views are important.</t>
-      </text>
-    </comment>
-    <comment ref="C58" authorId="150" shapeId="0" xr:uid="{DE897266-EE4C-430B-8A06-36671EA1ECF3}">
+    <comment ref="E57" authorId="2" shapeId="0" xr:uid="{7396887A-02AD-4130-B948-18DC9FEB21AA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst and assurer should enable and encourage peer review. Peer reviews provide useful critical challenge about the analytical approach, application of methods and interpretation of the analysis. Verification and peer review of work should be done by analysts who had no involvement in the work so their views are important.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C58" authorId="96" shapeId="0" xr:uid="{DE897266-EE4C-430B-8A06-36671EA1ECF3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2309,16 +2501,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E58" authorId="151" shapeId="0" xr:uid="{CE50D758-78EF-47CB-8DEF-6F69EB386D92}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst must determine and communicate the uncertainty associated with the analysis so the commissioner can make informed decisions. The commissioner should ensure that an assessment of uncertainty has been provided and that the implications of uncertainty are understood.
-</t>
-      </text>
-    </comment>
-    <comment ref="C59" authorId="152" shapeId="0" xr:uid="{D9DCD7D3-EAA6-44D2-9A62-38FD88896CA6}">
+    <comment ref="E58" authorId="2" shapeId="0" xr:uid="{9F454209-EAD8-4966-8974-0689A90A08F1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst must determine and communicate the uncertainty associated with the analysis so the commissioner can make informed decisions. The commissioner should ensure that an assessment of uncertainty has been provided and that the implications of uncertainty are understood.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C59" authorId="97" shapeId="0" xr:uid="{D9DCD7D3-EAA6-44D2-9A62-38FD88896CA6}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2342,16 +2538,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E59" authorId="153" shapeId="0" xr:uid="{057CF385-84BB-476C-8E6A-3FB469600EB4}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    If uncertainty is too complex to quantify, even approximately, the analysts should explain this so the commissioner can take this into account. In communicating analysis results to decision-makers and stakeholders, the commissioner should be open about the existence of deep uncertainties whose impact cannot be assessed, and explain how they are managed in the analysis.
-</t>
-      </text>
-    </comment>
-    <comment ref="C60" authorId="154" shapeId="0" xr:uid="{CF92684F-E55A-4187-96EE-68B56028E8CB}">
+    <comment ref="E59" authorId="2" shapeId="0" xr:uid="{878B7BD9-61C4-444A-AA56-6DCC07427376}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>If uncertainty is too complex to quantify, even approximately, the analysts should explain this so the commissioner can take this into account. In communicating analysis results to decision-makers and stakeholders, the commissioner should be open about the existence of deep uncertainties whose impact cannot be assessed, and explain how they are managed in the analysis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C60" authorId="98" shapeId="0" xr:uid="{CF92684F-E55A-4187-96EE-68B56028E8CB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2373,15 +2573,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E60" authorId="155" shapeId="0" xr:uid="{D3ECDD38-55DB-42AB-8E24-820D4D27690A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst must produce appropriate design documentation. Best practice includes maintaining a record of the analysis workflow in a technical report, including a concept of analysis, user requirements, design specification, functional specification, data dictionary, and test plan. Code should be properly documented.</t>
-      </text>
-    </comment>
-    <comment ref="C61" authorId="156" shapeId="0" xr:uid="{9626EEC2-270C-466A-BD46-FE28335E7E02}">
+    <comment ref="E60" authorId="2" shapeId="0" xr:uid="{7304F084-E09C-4B86-819B-DBCCD8639D29}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst must produce appropriate design documentation. Best practice includes maintaining a record of the analysis workflow in a technical report, including a concept of analysis, user requirements, design specification, functional specification, data dictionary, and test plan. Code should be properly documented.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C61" authorId="99" shapeId="0" xr:uid="{9626EEC2-270C-466A-BD46-FE28335E7E02}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2404,15 +2609,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E61" authorId="157" shapeId="0" xr:uid="{B275DA7B-24DD-46C5-BFD9-1B44FB5FAD46}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The analyst must produce appropriate documentation. Best practice includes maintaining a record of the work that has been done in a technical report, including a full description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer makes sure that the documentation is fit for purpose.</t>
-      </text>
-    </comment>
-    <comment ref="M61" authorId="158" shapeId="0" xr:uid="{60702B3D-0D4B-4988-B5E8-6A4A2C81D30B}">
+    <comment ref="E61" authorId="2" shapeId="0" xr:uid="{EE44CAB6-E9FE-43BE-9A9E-5D1837EFA660}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>The analyst must produce appropriate documentation. Best practice includes maintaining a record of the work that has been done in a technical report, including a full description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The assurer makes sure that the documentation is fit for purpose.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M61" authorId="100" shapeId="0" xr:uid="{60702B3D-0D4B-4988-B5E8-6A4A2C81D30B}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2421,7 +2631,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="C62" authorId="159" shapeId="0" xr:uid="{6F99AFD3-CF32-4152-A912-1D04F8967B37}">
+    <comment ref="C62" authorId="101" shapeId="0" xr:uid="{6F99AFD3-CF32-4152-A912-1D04F8967B37}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2444,15 +2654,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="E62" authorId="160" shapeId="0" xr:uid="{AFF19133-139A-4414-B5BD-D26EEAE944C9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Analysts should develop and maintain analysis code in line with best practice. Code must comply with relevant policies and standards.</t>
-      </text>
-    </comment>
-    <comment ref="C63" authorId="161" shapeId="0" xr:uid="{7DC36BDD-540A-4B1E-9888-76142C106F90}">
+    <comment ref="E62" authorId="2" shapeId="0" xr:uid="{59CB9FC1-C6B0-4BD3-807D-6219D6318303}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analysts should develop and maintain analysis code in line with best practice. Code must comply with relevant policies and standards.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C63" authorId="102" shapeId="0" xr:uid="{7DC36BDD-540A-4B1E-9888-76142C106F90}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2475,12 +2690,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="E63" authorId="162" shapeId="0" xr:uid="{971985CC-EE2C-4CAC-B5F2-03489CB55C67}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    You can assess the usefulness of the analysis by getting feedback from users, stakeholders and other experts. Quality analysis should be free of prejudice or bias. The SRO and analysts should check that the analysis follows the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust).</t>
+    <comment ref="E63" authorId="2" shapeId="0" xr:uid="{5785CF6B-3819-416B-8BCC-CF89B0ACA013}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>You can assess the usefulness of the analysis by getting feedback from users, stakeholders and other experts. Quality analysis should be free of prejudice or bias. The approver and analyst should check that the analysis follows the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust).</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -2488,7 +2708,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="244">
   <si>
     <t>This guidance is an ALPHA draft. It is in development and we are still working to ensure that it meets user needs.</t>
   </si>
@@ -2860,15 +3080,9 @@
     <t>Who do you need to consult to make sure you meet the right user needs?</t>
   </si>
   <si>
-    <t xml:space="preserve">Analyst, Commissioner	</t>
-  </si>
-  <si>
     <t>How will you know you have answered the analysis question correctly?</t>
   </si>
   <si>
-    <t xml:space="preserve">Commissioner, Analyst	</t>
-  </si>
-  <si>
     <t>What is the estimated time and resource required to answer the analysis question (in months and FTE)?</t>
   </si>
   <si>
@@ -3043,18 +3257,9 @@
     <t>Is there a clear feedback mechanism so users can report back on the suitability of outputs?</t>
   </si>
   <si>
-    <t xml:space="preserve">Commissioner, Assurer	</t>
-  </si>
-  <si>
     <t>Analyst, Commissioner, Assurer</t>
   </si>
   <si>
-    <t xml:space="preserve">Assurer, Commissioner, Analyst	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner, Analyst, Assurer	</t>
-  </si>
-  <si>
     <t>Analyst, Assurer</t>
   </si>
   <si>
@@ -3064,9 +3269,6 @@
     <t>Commissioner, Analyst, Assurer</t>
   </si>
   <si>
-    <t xml:space="preserve">Analyst, Assurer	</t>
-  </si>
-  <si>
     <t>Assurer, Analyst, Commissioner</t>
   </si>
   <si>
@@ -3079,12 +3281,6 @@
     <t>Commissioner, Assurer, Analyst</t>
   </si>
   <si>
-    <t xml:space="preserve">Commissioner, Approver	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner, Approver, Analyst team	</t>
-  </si>
-  <si>
     <t>Analyst, Approver</t>
   </si>
   <si>
@@ -3239,6 +3435,15 @@
   </si>
   <si>
     <t xml:space="preserve">QUESTIONS updated for new Code of Practice 3 </t>
+  </si>
+  <si>
+    <t>Commissioner, Approver</t>
+  </si>
+  <si>
+    <t>Commissioner, Approver, Analyst team</t>
+  </si>
+  <si>
+    <t>Assurer, Commissioner, Analyst</t>
   </si>
 </sst>
 </file>
@@ -4589,9 +4794,6 @@
     <text xml:space="preserve">A clear understanding of the analysis question is critical. It helps your team to scope out requirements, understand the strengths and limitations of the analysis and make sure it is fit for purpose.
 If the question is not clear, you risk designing and delivering analysis which does not meet user needs. </text>
   </threadedComment>
-  <threadedComment ref="E3" dT="2024-08-14T14:22:03.40" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{E21B303B-A7CD-43D0-B7EA-D905F032D9A5}">
-    <text xml:space="preserve">The commissioner sets out the commission. They work with the analyst team to ensure that everyone has a common understanding of the problem. </text>
-  </threadedComment>
   <threadedComment ref="L3" dT="2024-08-29T13:58:37.57" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{B717D9AE-0604-44A0-8412-B2D09E13C4CC}">
     <text xml:space="preserve">What analytical question you are addressing? </text>
   </threadedComment>
@@ -4602,10 +4804,6 @@
     <text xml:space="preserve">Knowing why you need the analysis, what it is for and how it will be used will help you to understand the importance and impact of your work and how it supports decision making.
 It will also help you to make sure the analysis is fit for purpose and correctly answers the question. </text>
   </threadedComment>
-  <threadedComment ref="E4" dT="2024-08-23T09:13:35.09" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{493BD2CC-B01C-4431-A4D3-5FF34D608502}">
-    <text xml:space="preserve">The analyst must document the purpose of the analysis and the levels of quality and certainty that are needed to meet user requirements. The commissioner and analytical assurer make sure the analysis aligns with the stated purpose.
-</text>
-  </threadedComment>
   <threadedComment ref="L4" dT="2024-08-29T13:58:37.57" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{9CF26141-1975-4AF9-A051-D7457E18733E}">
     <text xml:space="preserve">What is the need for this analysis or statistical release? </text>
   </threadedComment>
@@ -4613,22 +4811,11 @@
     <text xml:space="preserve">Knowing how the work aligns with organisational priorities shows how it will fit with wider strategic objectives and why you should do the analysis now.
 It informs the level of assurance needed to confirm the work is fit for purpose. </text>
   </threadedComment>
-  <threadedComment ref="E5" dT="2024-08-23T09:13:42.38" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{87ABBA1D-1BFB-4597-950F-7EA7A2EF80B2}">
-    <text>The commissioner makes sure that key aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated. They also make sure there is proportionate governance in place to support the analysis and its role in the wider project or programme</text>
-  </threadedComment>
   <threadedComment ref="C6" dT="2024-09-02T09:03:08.32" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{FDBC8216-3E37-4E41-BCE3-4BA3377DA5C0}">
     <text>Identifying if the work is business critical determines the assurance needed to ensure it is fit for purpose.</text>
   </threadedComment>
-  <threadedComment ref="E6" dT="2024-08-23T09:13:53.81" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{8EB3435E-2AD8-4AF9-9477-10355940958D}">
-    <text xml:space="preserve">Business critical models must be managed appropriately so that the right specialists are responsible for developing, using and assuring them.
-Decision-makers need sufficient assurance from an appropriate level in the organisation that the model is fit for purpose before using it to inform a decision. For business critical analysis and modelling, the commissioner should be satisfied with the seniority of the analytical assurer. </text>
-  </threadedComment>
   <threadedComment ref="C7" dT="2024-09-02T09:03:15.72" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{BCCD1820-2B3B-4FEC-8B83-86DBCC941395}">
     <text>Knowing what your outputs will be used for can ensure they meet user needs. A good understanding of uses is essential for making sure that your analysis is fit for purpose.</text>
-  </threadedComment>
-  <threadedComment ref="E7" dT="2024-08-23T09:14:00.91" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{18A1EB84-066B-483A-A278-351D641106BE}">
-    <text xml:space="preserve">The commissioner makes sure that the right stakeholders have been identified so that the scope and boundaries of the analysis can be appropriately explored. The analyst team and analytical assurer should also contribute.
-</text>
   </threadedComment>
   <threadedComment ref="L7" dT="2024-08-29T13:58:37.57" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{BC3B8A1E-E152-4A66-BD49-D05803E09CA5}">
     <text xml:space="preserve">Who uses your analysis or statistical release?  </text>
@@ -4638,17 +4825,10 @@
 Identify relevant stakeholders and users, consult them before designing the analysis, and consider their views.
 Consulting the right stakeholders helps you and your users agree on how to answer the question and what the output should look like. This means you can check the users' understanding of the process and its quality, and that the final output meets user needs.</text>
   </threadedComment>
-  <threadedComment ref="E8" dT="2024-08-23T09:14:07.53" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{AA6BAEC1-9530-43AE-A233-E2E7C0374046}">
-    <text xml:space="preserve">Analysts should explore the analysis requirements and scope with all relevant stakeholders to make sure a wide range of perspectives are sought. The commissioner should be aware and briefed.
-</text>
-  </threadedComment>
   <threadedComment ref="C9" dT="2024-09-02T09:06:52.50" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{FB4107FF-85E4-4674-9C4E-7753AB019F16}">
     <text xml:space="preserve">Being clear about the outputs required and acceptable uncertainty is essential for producing accurate and reliable outputs where users understand the work's limitations and uncertainty.
 It is also essential when designing verification and validation activities to check the robustness of results under a range of plausible assumptions about methods and data. </text>
   </threadedComment>
-  <threadedComment ref="E9" dT="2024-08-23T09:14:17.91" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{EF364E4F-6B64-4BFB-8A60-041DE12319C2}">
-    <text>During the design and conduct of analysis, the commissioner should set out details like the level of precision, accuracy and uncertainty that are needed.</text>
-  </threadedComment>
   <threadedComment ref="L9" dT="2024-08-29T14:30:21.94" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{4D792EE8-5DFC-473C-9F60-5F342A95B67E}">
     <text xml:space="preserve">How do you know that your analysis or statistical process is working correctly? </text>
   </threadedComment>
@@ -4656,10 +4836,6 @@
     <text xml:space="preserve">Without a clear understanding of time and resources available, you may overcommit. It is important to push back against unrealistic demands if there is not enough time to effectively quality assure the analysis.
 The users and commissioner should fully understand and accept increased risks to quality when time and resource pressures are unavoidable. </text>
   </threadedComment>
-  <threadedComment ref="E10" dT="2024-08-23T09:14:50.86" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{4A376BBA-7716-405F-A998-FBDCCFB6D36A}">
-    <text xml:space="preserve">During commissioning and scoping, the commissioner and analyst will need to make trade-offs between time, resources and quality. They should work together to agree and document the right balance across these constraints.
-</text>
-  </threadedComment>
   <threadedComment ref="M10" dT="2024-08-29T13:38:23.38" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{297D13ED-C651-43E5-A296-C92BDF8140A0}">
     <text xml:space="preserve">How much time does your statistics output take to produce and how is this time split between data collection, analysis, report preparation and QA? Does the current balance feel effective?
 </text>
@@ -4667,29 +4843,17 @@
   <threadedComment ref="C11" dT="2024-09-02T09:07:07.16" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B8611E4F-62CB-4E5B-B541-B7D57EDFE31B}">
     <text>Understanding why the work needs to happen now will help you to prioritise and use limited resources for the right activities.</text>
   </threadedComment>
-  <threadedComment ref="E11" dT="2024-08-23T09:15:00.34" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{91DA7871-3F83-489C-9B2C-D097153E5C8B}">
-    <text>The commissioner makes sure that there is sufficient time and resource for the required level of assurance to be delivered and that they understand the risks when time and resource pressures are unavoidable.</text>
-  </threadedComment>
   <threadedComment ref="C12" dT="2024-09-02T09:07:17.24" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{DDA67DCB-8363-4F2A-8E2F-D7FD31758CC8}">
     <text xml:space="preserve">Understanding the possible legal, financial or reputational consequences if the analysis is not carried out correctly helps you to design proportionate assurance activities.
 You should consider how these consequences line up with the risk appetite of your organisation when you design your mitigation. </text>
   </threadedComment>
-  <threadedComment ref="E12" dT="2024-08-23T09:15:06.23" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{0229EB7C-8A73-4B9E-9D13-796DEAA70543}">
-    <text>The commissioner makes sure the analyst team understands the context for the analysis question. This helps the analyst to understand and assess likely risks and determine the right analytical and quality assurance response.</text>
-  </threadedComment>
   <threadedComment ref="C13" dT="2024-09-02T09:07:25.20" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{4EFF044A-661A-45F8-9173-7EAF843C1921}">
     <text>Clear accountability makes sure that important decisions are signed off by the right people. There should be a clear understanding of who is responsible for managing, producing and quality assuring the analysis in the team.</text>
-  </threadedComment>
-  <threadedComment ref="E13" dT="2024-08-23T09:15:13.95" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{0B3233E4-B736-4C2D-AADA-A0925FF322D3}">
-    <text>During scoping of the analysis, the commissioner makes sure there is proportionate governance in place to support the analysis and its role in the wider project or programme.</text>
   </threadedComment>
   <threadedComment ref="C14" dT="2024-09-02T09:07:34.53" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B074A2B9-B46E-4830-BCD5-A7D9FC9F80B3}">
     <text>Before starting, identify all the skills and resources needed to produce the final output in a sustainable and reproducible way and quality assure it at every step.
 The platform used to host the analysis and the software to build and run the analysis should be appropriate and risks considered. For example, producing critical outputs in Excel does not comply with best practice and is unlikely to be robust or verifiable.</text>
   </threadedComment>
-  <threadedComment ref="E14" dT="2024-08-23T09:15:22.24" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{F49D43AA-2830-4C6A-B1BB-5F30B710381C}">
-    <text>The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</text>
-  </threadedComment>
   <threadedComment ref="M14" dT="2024-08-29T12:47:32.51" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{14C4500A-297B-4DC2-A81E-5404A0E6855E}">
     <text xml:space="preserve">What analytical tools do you use during the production process? Are they the best for the job?
 </text>
@@ -4697,16 +4861,10 @@
   <threadedComment ref="C15" dT="2024-09-02T09:07:42.56" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{BDD5D421-F6F7-4018-BBB9-CC062F53505D}">
     <text>If the team lacks capability, resource, or time, this increases the risk that the analysis will not be fit for purpose or sufficiently assured.</text>
   </threadedComment>
-  <threadedComment ref="E15" dT="2024-08-23T09:15:30.32" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{A8911257-2BC7-4D42-BB6B-8A505C0946B1}">
-    <text>The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.</text>
-  </threadedComment>
   <threadedComment ref="C16" dT="2024-09-02T09:07:52.90" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{675351E7-4AAD-4CAE-A63B-A1432693D85A}">
     <text xml:space="preserve">You must identify potential risks and their impact well in advance to enable effective mitigation and quicker, confident decision-making.
 It is important that users understand risks to ensure that their expectations and requirements are met. You should document how you have identified and are monitoring and mitigating risks. </text>
   </threadedComment>
-  <threadedComment ref="E16" dT="2024-08-23T09:15:39.30" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{16B73972-A012-48B7-A793-DAD887DBB3BF}">
-    <text>The analystical assurer should challenge and test the understanding of the problem. The commissioner and analyst work with the analytical assurer to make sure that all share a common understanding.</text>
-  </threadedComment>
   <threadedComment ref="M16" dT="2024-08-29T13:35:36.92" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{247C10C3-5E6D-4D86-B576-9EA0227FA976}">
     <text xml:space="preserve">Where are the highest risk points for errors in the process? What measures do you or could you take to mitigate risk at these points?
 </text>
@@ -4714,34 +4872,17 @@
   <threadedComment ref="C17" dT="2024-09-02T09:08:00.76" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{8ACF04DB-3056-4F30-B39E-A41DFC39BAD7}">
     <text>You should account for risks that you can mitigate. Include risks that have a high impact on the analysis but a low probability happening. Without well designed contingencies, we put quality at risk.</text>
   </threadedComment>
-  <threadedComment ref="E17" dT="2024-08-23T09:15:52.94" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{38227814-F8B1-46EF-ABEB-7DEC64C60144}">
-    <text xml:space="preserve">The commissioner makes sure that there is enough time and resource for the required level of assurance to be delivered. They must be confident that they understand the risks when time and resource pressures are unavoidable.
-If there is a need for urgent action, such as mitigation of unacceptable but uncertain risks, the commissioner may ask for further analysis. They might also commission extra evidence-gathering in parallel to inform the policy response when uncertainty is reduced. The analytical assurer must advise the commissioner on whether sufficient analytical quality assurance has happened and inform them about any outstanding risks. </text>
-  </threadedComment>
   <threadedComment ref="C18" dT="2024-09-02T09:08:09.45" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{59656D8A-69E5-4CDB-8CA0-48493A72EB6E}">
     <text>Analysis must comply with ethics standards to ensure public confidence. You must consider the ethical implications of the analysis when you create the workflow and report your findings.</text>
   </threadedComment>
-  <threadedComment ref="E18" dT="2024-08-23T09:16:00.75" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{65E6E0EC-BC6A-4935-A14C-FBA6D651D1C0}">
-    <text>The analyst should make sure that there is appropriate ethical approval for the analysis. The commissioner and analytical assurer should be informed.</text>
-  </threadedComment>
   <threadedComment ref="C19" dT="2024-09-02T09:08:27.58" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{6326AB4D-3C57-460D-B340-3271BFEA81A2}">
     <text>Limiting the scope of analysis shapes the quality of outputs and what can be done with them. By being clear about the limitations of the analysis we can mitigate or accept them. Limitations must be documented so everybody using the analysis is aware of them.</text>
   </threadedComment>
-  <threadedComment ref="E19" dT="2024-08-23T09:16:08.57" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{E0E21280-EAE1-4A23-948F-48D7D64315E4}">
-    <text xml:space="preserve">The commissioner and the analyst work together at the scoping stage to get a clear understanding of analytical requirements. During scoping, the commissioner makes sure that the right aspects of the problem, scope and complexities, including programme constraints, are captured and clearly communicated.
-</text>
-  </threadedComment>
   <threadedComment ref="C20" dT="2024-09-02T09:08:38.75" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{C2A9A967-BCAA-453B-9DE1-A1889DA749F8}">
     <text>Internal audit and peer review are critical for monitoring and assuring that the analysis is performed appropriately and meets the required aims and objectives. The outcomes of peer review should be documented and relevant actions and recommendations should be prioritised, addressed, and taken forward.</text>
   </threadedComment>
-  <threadedComment ref="E20" dT="2024-08-23T09:16:17.18" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{5BC7BB64-C399-4C88-910A-EE0A196D541B}">
-    <text>The analytical assurer makes sure quality assurance plans for the analysis are appropriate for the decision it supports. All analysis requires some level of quality assurance. Analyst and commissioner should be involved.</text>
-  </threadedComment>
   <threadedComment ref="C21" dT="2024-09-02T09:08:46.72" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{71D7AD01-61DA-4F82-B9B6-13FA8081889E}">
     <text>You should commission external specialists to peer review or audit the analysis in proportion to risks around use. They should be able to draw on expertise and experience across government and beyond to get feedback, exchange experience and suggest best practice to improve the analysis.</text>
-  </threadedComment>
-  <threadedComment ref="E21" dT="2024-08-23T09:16:58.24" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{94791D6F-A09E-4058-A847-C891B2C626C4}">
-    <text>The analytical assurer should challenge the proposed approach. Check that it delivers as intended and meets customer needs. It is good practice to engage subject matter experts in this review. Analyst and commissioner should be involved.</text>
   </threadedComment>
   <threadedComment ref="M21" dT="2024-08-29T13:34:07.61" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{2711FEBA-50F1-49C4-BBCD-00FD8773322F}">
     <text xml:space="preserve">Is your code or analysis ever peer reviewed by someone outside your team or organisation?
@@ -4751,18 +4892,10 @@
     <text xml:space="preserve">Writing a plain English description of what the analysis is for and how it works means that everybody in the team, including new starters, and others with no subject or technical expertise can understand the purpose of the analysis and what it does.
 </text>
   </threadedComment>
-  <threadedComment ref="E22" dT="2024-08-23T09:36:18.12" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{816A930F-38AC-4BF9-B788-9577B0D60F19}">
-    <text xml:space="preserve">The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer should give feedback to make sure documentation is fit for purpose.
-</text>
-  </threadedComment>
   <threadedComment ref="C23" dT="2024-09-02T09:09:34.81" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{1F0E8DDD-3806-4EB2-A559-E138AD955876}">
     <text xml:space="preserve">Setting out a clear summary of the analysis process in a diagram helps the team, users and customers to understand at a glance what the analysis does, where inputs come from, how they are processed and how it generates outputs.
 </text>
   </threadedComment>
-  <threadedComment ref="E23" dT="2024-08-23T09:36:25.03" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{13E8362D-B596-42DC-A9CB-A062A4B94158}">
-    <text xml:space="preserve">The analyst should produce sufficient design documentation. Best practice can include a description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer should give feedback to make sure documentation is fit for purpose.
-</text>
-  </threadedComment>
   <threadedComment ref="L23" dT="2024-08-29T14:06:53.90" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{5EB69C75-C40A-4B3C-A1C9-C76AB1F55EF6}">
     <text xml:space="preserve">Can you summarise and explain the end-to-end process of your analysis or statistical release for somebody who asks about it? </text>
   </threadedComment>
@@ -4773,10 +4906,6 @@
   <threadedComment ref="C24" dT="2024-09-02T09:09:42.68" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{41BE326F-BE7B-4F34-83F1-BA0897CC104B}">
     <text>Clearly setting out the time you need to perform each stage of analysis helps you to evaluate if the time allocated to each stage is right and plan mitigation if plans look too ambitious.</text>
   </threadedComment>
-  <threadedComment ref="E24" dT="2024-08-23T09:36:31.72" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{278AF0F5-1106-492A-AB60-8B0CBF7DA4D5}">
-    <text xml:space="preserve">The analyst and commissioner should work together during scoping to set out and agree trade-offs between time, resources and quality and establish the optimal balance of these constraints.
-</text>
-  </threadedComment>
   <threadedComment ref="M24" dT="2024-08-29T12:43:41.53" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{CF291131-C014-40E1-8BDC-CE14CA286B85}">
     <text xml:space="preserve">How much time does your statistics output take to produce and how is this time split between data collection, analysis, report preparation and QA? Does the current balance feel effective?
 </text>
@@ -4785,10 +4914,6 @@
     <text xml:space="preserve">Manual processes are inefficient and more risky than well-designed automated ones. Analysis with manual steps like copying and pasting data between files, manually updating cells in tables, or moving data between software packages is harder to assure and carries extra quality risks.
 </text>
   </threadedComment>
-  <threadedComment ref="E25" dT="2024-08-23T09:37:24.21" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{A8AE3539-0828-48D7-85A6-95E81786F997}">
-    <text xml:space="preserve">The analyst should use a risk-based approach to understand the areas of greatest potential error and focus assurance efforts on these areas. The analyst should brief the commissioner so they understand the impact of any reduction in the thoroughness of analytical quality assurance activities.
-</text>
-  </threadedComment>
   <threadedComment ref="M25" dT="2024-08-29T12:50:38.13" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{75DDAEFF-7FE9-48F4-B766-4CAA33B2B677}">
     <text xml:space="preserve">How many manual steps are there in the process (e.g. updating cells in spreadsheets, moving data between software or copy-paste steps)? Could these be reduced to minimise the risk of error?
 </text>
@@ -4801,10 +4926,6 @@
     <text xml:space="preserve">Mistakes happen in analysis. You should have a clear and efficient process for reporting, documenting and addressing errors. Being open and honest about problems and working together to solve them in a supportive way creates an atmosphere of openness in the team and is critical for upholding users’ trust in your output.
 Teams should take reasonable steps to understand and document how and why errors came about, and mitigate the risk of them happening again. Your mitigation approach should be consistent with your department’s revision policies. </text>
   </threadedComment>
-  <threadedComment ref="E26" dT="2024-08-23T09:37:32.12" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{A42575B9-C972-453B-8A32-9A671BEDE603}">
-    <text xml:space="preserve">The analyst should use a risk-based approach to highlight the areas of greatest potential error and focus assurance efforts on these areas.
-</text>
-  </threadedComment>
   <threadedComment ref="L26" dT="2024-08-29T14:09:25.76" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{A312EA72-F9CB-4C05-8E8D-7D66458CCD38}">
     <text xml:space="preserve">If you find a mistake in your analysis, do you have a clear and efficient process for addressing the issue and preventing it from happening again? </text>
   </threadedComment>
@@ -4820,42 +4941,25 @@
     <text xml:space="preserve">Consider how uncertainty impacts on all stages of the analysis. Think about quantifying and measuring uncertainty as early as possible. Identify and review sources of uncertainty regularly.
 If you delay the assessment of uncertainty until late in the process, it is often difficult and costly to mitigate risks. In some cases, you may need to revise methods or alter commissioning decisions. If a potential source of uncertainty is overlooked, this can limit the usefulness and impact of the analysis. </text>
   </threadedComment>
-  <threadedComment ref="E27" dT="2024-08-23T09:37:40.59" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{FF90D25A-4F6A-4F0E-A1D7-85C575ABF4CF}">
-    <text xml:space="preserve">Commissioners should expect and require information about uncertainty from analysts. They should challenge them when it is absent, inadequate or ambiguous.
-Commissioners may have identified sources of uncertainty as part of their wider considerations and should share them with the analyst. If the commissioner can explain in advance the impact on decision-making of different degrees of uncertainty, this can help the analyst to design and carry out the analysis at a proportionate level. </text>
-  </threadedComment>
   <threadedComment ref="L27" dT="2024-08-29T14:20:20.61" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{8680581D-D8CB-43C2-9441-DEA37E980EB7}">
     <text xml:space="preserve">How do you measure and report uncertainty in your analysis or statistical release? </text>
   </threadedComment>
   <threadedComment ref="C28" dT="2024-09-02T09:16:17.59" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D988F73F-692A-43EF-A4EA-3CD1684C9B6D}">
     <text>Processing the data inputs will impact methods and outputs. A clear understanding of how these processes affect the workflow is essential for understanding quality.</text>
   </threadedComment>
-  <threadedComment ref="E28" dT="2024-08-23T10:04:28.37" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{1B01FECE-7BE0-4343-BCCC-DAEB90C40E6F}">
-    <text xml:space="preserve">The analyst should collect and manage the data. They must understand data accuracy and uncertainties and capture, manage and understand assumptions. Analytical assurer should check that data processing is sufficient to ensure fitness for purpose.
-</text>
-  </threadedComment>
   <threadedComment ref="C29" dT="2024-09-02T09:16:24.21" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{1F976AE5-334F-44B3-8203-575633C5DBA1}">
     <text>A comprehensive understanding of data inputs is a prerequisite for meeting user needs.</text>
-  </threadedComment>
-  <threadedComment ref="E29" dT="2024-08-23T10:04:38.86" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{33FFCD26-892E-48CB-9570-5772ACF052DA}">
-    <text>The analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The analyst should engage appropriate subject matter experts at the appropriate time. The commissioner may be a subject matter expert. The analytical assurer should check that there is sufficient assurance around the choice of data.</text>
   </threadedComment>
   <threadedComment ref="C30" dT="2024-09-02T09:16:36.91" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{AE45F985-AF8D-42E4-9B36-D04CCB025BDC}">
     <text xml:space="preserve">Data requirements for analysis vary. Formats, coverage, time scales and granularity must all be appropriate for the research question.
 A comprehensive understanding of data inputs is a prerequisite for meeting user needs. Without understanding the strengths and weaknesses of the data, it is impossible to make meaningful improvements to the analysis or the inputs to manage these limitations. </text>
   </threadedComment>
-  <threadedComment ref="E30" dT="2024-08-23T10:04:49.69" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{AFCA1F9F-3656-4D87-B028-158FAC82491A}">
-    <text>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. Analytical assurer should make sure there is sufficient consideration of strengths and limitations of data.</text>
-  </threadedComment>
   <threadedComment ref="L30" dT="2024-08-29T13:59:43.62" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{D5F09098-7F1D-4BB7-A6B2-A1BA1A704874}">
     <text xml:space="preserve">What is the quality of the data that you use? </text>
   </threadedComment>
   <threadedComment ref="C31" dT="2024-09-02T09:16:44.28" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{CE1E2D36-2C45-4BCE-AE89-C30A66B393BE}">
     <text xml:space="preserve">A good relationship with data suppliers helps to make sure that their data meet your requirements. Lack of communication can mean you are not aware of quality risks or changes in collection or processing steps that can affect your results.
 You should communicate with your suppliers sufficiently to manage input quality. Data providers should have a good understanding of how and why you are using their data. This helps them to improve data quality and value and find and address gaps or issues that are relevant for your analysis. </text>
-  </threadedComment>
-  <threadedComment ref="E31" dT="2024-08-23T10:05:05.00" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{1D6C5D70-BF17-4EEC-B30F-90C6BA3581C9}">
-    <text>The analytical assurer should expect to see evidence that there has been sufficient dialogue between analysts and the providers of data and other evidence sources.</text>
   </threadedComment>
   <threadedComment ref="M31" dT="2024-08-29T12:56:42.88" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{94FFD0A4-94E6-44D0-AFF1-E4D74A4A55C2}">
     <text xml:space="preserve">When and how do you communicate with your data provider(s)?
@@ -4865,16 +4969,10 @@
   <threadedComment ref="C32" dT="2024-09-02T09:16:50.35" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{6C1003AE-3D74-420B-93F3-9EB78C864F06}">
     <text>Never assume that datasets are of sufficient quality. Make sure that suppliers give you the metadata and other supporting information you need to assure the quality of the data. Validate the information provided by suppliers using your own checks and confirmation if appropriate.</text>
   </threadedComment>
-  <threadedComment ref="E32" dT="2024-08-23T10:05:15.38" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{352754FD-B656-49F3-BCAA-2FFE4A505A14}">
-    <text>The analyst should ensure data formats, units, and context are properly understood and handled. They should design and implement quality checks to validate data inputs as required. Analytical assurer should verify that the right assurance is in place.</text>
-  </threadedComment>
   <threadedComment ref="C33" dT="2024-09-02T09:16:56.86" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{59EC36DA-6B9E-413F-89C4-56E9E7E44A89}">
     <text xml:space="preserve">A formal service level agreement with data providers makes sure that everybody understands what will be delivered, when and how. This is useful for setting out the division of responsibilities between data providers and your team for getting and sharing the data. It might specify formats, delivery, timescale, legal framework, accompanying metadata and quality checks.
 </text>
   </threadedComment>
-  <threadedComment ref="E33" dT="2024-08-23T10:05:25.40" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{9D913C7D-0166-4537-882F-9848E15DAC6B}">
-    <text>The commissioner may need to provide the analyst with agreement to use specific data. The analyst should ensure data formats, units, and context are properly understood and handled. Analytical assurer should verify that assurance is in place.</text>
-  </threadedComment>
   <threadedComment ref="M33" dT="2024-08-29T12:57:44.35" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{24B80C75-97C1-4F68-8BB1-DE33FF04E0FD}">
     <text xml:space="preserve">Is there a formal agreement in place that specifies when, what and how the data will be received? If not, do you think this would be helpful?
 </text>
@@ -4883,9 +4981,6 @@
     <text xml:space="preserve">Data suppliers should be able to show that their data is sufficiently assured to meet your needs. You should be able to demonstrate that the data meet your needs and that reported quality matches what you observe in practice. Simply having a quality report is not enough.
 </text>
   </threadedComment>
-  <threadedComment ref="E34" dT="2024-08-23T10:05:34.49" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{789F6E67-B991-40BF-9F64-84F8CAAC5041}">
-    <text>The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The analytical assurer should assess whether assurance is sufficient.</text>
-  </threadedComment>
   <threadedComment ref="M34" dT="2024-08-29T12:58:24.73" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{68906487-86CE-4423-968E-A85B0B386C25}">
     <text xml:space="preserve">Do you know what quality checks are carried out on the data before you receive them?
 </text>
@@ -4894,10 +4989,6 @@
     <text xml:space="preserve">Review your data requirements regularly to ensure they are still relevant and feasible. Changes to requirements should be communicated to data providers well in advance and agreed by all stakeholders. If there is a formal agreement, it may need to be revised as requirements change.
 </text>
   </threadedComment>
-  <threadedComment ref="E35" dT="2024-08-23T10:05:43.11" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{720155DB-43E9-4E3D-B067-80E33979909F}">
-    <text xml:space="preserve">During the design and conduct of analysis, the commissioner may need to provide the analyst with information, agreement to use resources or confirmation of assumptions or approach. The analyst should understand data accuracy and uncertainties and capture, manage and understand implicit assumptions made. The analytical assurer checks that assurance and mitigation are sufficient.
-</text>
-  </threadedComment>
   <threadedComment ref="M35" dT="2024-08-29T12:59:15.19" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{6EF05AFF-6624-4C00-B17D-CDF5A0D6B9A2}">
     <text xml:space="preserve">How do you work with your data provider when your data requirements change?
 </text>
@@ -4905,10 +4996,6 @@
   <threadedComment ref="C36" dT="2024-09-02T09:17:24.04" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{BB6FCFEC-05A0-43EC-9122-0C14DAE7A149}">
     <text>Data suppliers make changes to their definitions, methods and systems. This may not affect the quality of their data but can affect how you process the data and what you can infer from it. Tailor communication with data suppliers so it is sufficiently frequent, effective and ongoing to get timely information about changes.</text>
   </threadedComment>
-  <threadedComment ref="E36" dT="2024-08-23T10:05:55.32" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{BA304E9A-5542-409A-B97D-1C87720091F2}">
-    <text xml:space="preserve">During the design and conduct of analysis, the commissioner provides the analyst with the information they need for the analysis to proceed. This could include agreement to use datasets, setting out of key assumptions and signing off assumptions developed during the project. Analyst should understand data accuracy and uncertainties and capture, manage and understand assumptions made. The analytical assurer checks that assurance and mitigation are sufficient.
-</text>
-  </threadedComment>
   <threadedComment ref="M36" dT="2024-08-29T12:59:41.86" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{81C63929-92E1-4141-AC89-6265FEF8F817}">
     <text xml:space="preserve">How do you know if your data provider makes a change to their systems or processes, which could impact the data you receive and/or the statistics you produce?
 </text>
@@ -4916,9 +5003,6 @@
   <threadedComment ref="C37" dT="2024-09-02T09:18:25.68" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{C592D865-BAF0-40E5-B06F-95DD894CCD3E}">
     <text>You should be able to explain why you chose your methods. For each method, document the underlying assumptions, why the method is suitable for answering the analysis question, why it is applicable to the type and distribution of data you are using, and how these decisions were signed off.</text>
   </threadedComment>
-  <threadedComment ref="E37" dT="2024-08-23T10:06:10.96" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{161293C4-3808-44F5-87D0-3A58D1DCE9F9}">
-    <text>During the design phase, the analyst will convert the commission into an analytical plan and will consider inputs, analytical methods and processes, and expected outputs. The analytical assurer should check that the proposed design meets the commissioner’s requirements and is sufficiently assured.</text>
-  </threadedComment>
   <threadedComment ref="L37" dT="2024-08-29T14:00:09.29" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{9CBE22E1-DFBF-48CA-BB5A-4DF7E0890029}">
     <text xml:space="preserve">How did you choose the methods for the analysis or statistical release? </text>
   </threadedComment>
@@ -4928,15 +5012,8 @@
   <threadedComment ref="C38" dT="2024-09-02T09:18:35.11" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{0E1ABA66-3073-40B5-A07B-B302C405B9DC}">
     <text>There is often more than one way to answer a question with data. When you have made choices about methods and approaches, explain how and why you considered and rejected other options. Unless there is evidence underpinning your choice, users cannot be sure that you have chosen the most suitable methods.</text>
   </threadedComment>
-  <threadedComment ref="E38" dT="2024-08-23T10:06:17.40" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{13691A62-9845-4A10-BED2-EA476C092F84}">
-    <text xml:space="preserve">The analyst should review the analysis as a whole and consider carefully whether there are other, better ways in which it could be done. The analytical assurer should check that the investigation of methods was sufficiently thorough and proportionate.
-</text>
-  </threadedComment>
   <threadedComment ref="C39" dT="2024-09-02T09:18:43.17" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{4C4EB5D3-295C-4C4C-BCEB-F7E54CBF6B44}">
     <text>You need to be sure that your analysis produces the outputs you think it should and the processes run as expected. If you cannot demonstrate that scripts and processes work correctly, you cannot confirm the quality of the results.</text>
-  </threadedComment>
-  <threadedComment ref="E39" dT="2024-08-23T10:06:24.70" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D7DFEC19-E955-4AFD-9AAC-0E883202371E}">
-    <text>The analyst should validate that the analysis as set up to answer the specification of the commissioner. The analytical assurer checks that assurance and mitigation are sufficient so the analysis is fit for purpose.</text>
   </threadedComment>
   <threadedComment ref="L39" dT="2024-08-29T14:07:51.19" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{6A84BEE9-C34F-407C-A8FF-1723B8A09754}">
     <text xml:space="preserve">How do you know that your analysis or statistical process is working correctly? </text>
@@ -4953,59 +5030,31 @@
     <text xml:space="preserve">You must understand the assumptions your analysis makes. Assumptions set out how the analysis simplifies the world and mitigates uncertainty. If assumptions are inadequately set out or absent, important characteristics of the analysis and its inputs will be unclear, greatly increasing risk.
 Without a comprehensive log of assumptions made by the analysis, an audit trail signed off by assumption owners, a version control log reflecting when assumptions were last updated, and evidence showing internal and external validation of assumptions, uncertainties may go unacknowledged and could drastically impact outputs. </text>
   </threadedComment>
-  <threadedComment ref="E40" dT="2024-08-23T10:06:31.30" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{78EB6020-989C-48A3-BE00-A20C1EC63773}">
-    <text xml:space="preserve">The analyst should capture, manage and understand explicit and implicit assumptions made. The analytical assurer should assess whether these are sufficient. The commissioner should be made aware of key assumptions and confirm that they are happy that the assumptions are applied.
-</text>
-  </threadedComment>
   <threadedComment ref="C41" dT="2024-09-02T09:19:02.64" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{FA0D8310-A90C-42E4-9210-CD9B57782310}">
     <text>A clear understanding of how assumptions have been externally and internally validated and signed off gives us confidence that they are reasonable.</text>
-  </threadedComment>
-  <threadedComment ref="E41" dT="2024-08-23T10:06:55.06" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{AEA4B76B-7193-4905-A4F4-A5B6D6DD5251}">
-    <text>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain assumptions. Analytical assurer should check that validation and assurance of assumptions is sufficient.</text>
   </threadedComment>
   <threadedComment ref="C42" dT="2024-09-02T09:19:12.44" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{E0879D79-098E-41CF-95EB-C39AE1D0159B}">
     <text xml:space="preserve">All analysis contains uncertainty. Quantifying and reporting uncertainty means we can inform users how precise reported values are and how much confidence they can have in the analysis. It will also help you to determine where the analysis can be improved.
 There are many ways to quantify uncertainty in input data, assumptions, processes and outputs. Choose appropriate ones for your situation. For instance, uncertainties can be understood and quantified by comparing against similar or historical data, Monte Carlo simulation, break-even analysis or using expert judgement. </text>
   </threadedComment>
-  <threadedComment ref="E42" dT="2024-08-23T10:07:06.86" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D80C5B0D-CFEF-499C-868E-94EAB93E723B}">
-    <text xml:space="preserve">Analyst should determine and communicate the uncertainty associated with outputs so that the commissioner can make informed decisions. The range of possible outcomes and their relative likelihoods should be described. The analytical assurer checks that measuring and reporting of uncertainty is sufficient to meet the needs of the commissioner.
-</text>
-  </threadedComment>
   <threadedComment ref="L42" dT="2024-08-29T14:13:12.62" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{A3AE9B5E-0310-4350-9807-69ABC66B6211}">
     <text xml:space="preserve">How do you measure and report uncertainty in your analysis or statistical release? </text>
   </threadedComment>
   <threadedComment ref="C43" dT="2024-09-02T09:19:19.77" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{5D7453CB-76BE-40D2-B145-19184CD3A890}">
     <text>A good understanding of the uncertainties in the analysis workflow is critical to ensure the analysis and its outputs are fit for purpose.</text>
-  </threadedComment>
-  <threadedComment ref="E43" dT="2024-08-23T10:08:50.10" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{060CC347-F854-423E-9201-C561757B4AD3}">
-    <text>If uncertainties are too complex for analysts to quantify, even approximately, the analysts should say so in order that the commissioner can take this into account.</text>
   </threadedComment>
   <threadedComment ref="C44" dT="2024-09-02T09:19:30.21" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{4726F164-972F-4AA8-9C1B-1471585CA560}">
     <text xml:space="preserve">Understanding how your analysis might be used would help ensure that the right quality and assurance levels are in place. It would help you assess the risks around the use of analysis and if there are other stakeholders or users you need to consult.
 </text>
   </threadedComment>
-  <threadedComment ref="E44" dT="2024-08-23T10:09:01.94" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{695704F7-9606-4A5A-A932-B8C892921EF8}">
-    <text xml:space="preserve">Analyst should make sure that the implications of data dependencies or relationships to other analysis and methods are understood. Analytical assurer should check that dependencies have been properly considered.
-</text>
-  </threadedComment>
   <threadedComment ref="C45" dT="2024-09-02T09:19:39.11" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B7BA39CD-9FF1-46C7-A57F-300A0D0CA61F}">
     <text>Single points of failure carry significant business risk. If only one person understands how to carry out all or part of the analysis or maintain the code then the process is extremely vulnerable.</text>
   </threadedComment>
-  <threadedComment ref="E45" dT="2024-08-23T10:09:15.67" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B73FA1FF-4A86-442A-8939-1EB1B3637BC1}">
-    <text>Analysis should be peer reviewed at an appropriate and proportionate level by a competent person. Commissioner, analyst and analytical assurer should all be involved in each stage of the analytical cycle.</text>
-  </threadedComment>
   <threadedComment ref="C46" dT="2024-09-02T09:19:49.02" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{61AF9F9A-52A3-4A72-A307-527A48F4FF97}">
     <text>All analysis involves decisions. A comprehensive record of the decisions made in specifying and conducting the analysis ensures a full audit trail of why decisions were made, who made them and signed them off.</text>
   </threadedComment>
-  <threadedComment ref="E46" dT="2024-08-23T10:09:26.86" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B9EF0E84-E789-47B4-A769-C8B7107137C0}">
-    <text>The analytical assurer should make sure that a suitable audit trail is in place that clarifies the level of validation, scope, and risks associated with the analysis. Best practice includes the production of validation log books. Analyst should build this audit trail.</text>
-  </threadedComment>
   <threadedComment ref="C47" dT="2024-09-02T09:22:17.51" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{6A948CD1-63AD-457F-B394-1F7D35C4BE64}">
     <text>Good version control ensures a full understanding of when, why, and how changes were made to your analysis process. If it is hard to track changes, it will be hard to retrace steps if there is a problem and means you do not fully understand the process.</text>
-  </threadedComment>
-  <threadedComment ref="E47" dT="2024-08-23T10:09:39.80" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{F8A8E0E6-D628-47A5-9AFE-D12B9730A1D9}">
-    <text xml:space="preserve">To make analytical audit easy, you should set up a version control system for the analysis as a whole and for code, supporting data and assumptions. Best practice includes the production of validation log books. Analyst should build this audit trail. The Analytical assurer should ensure that the audit trail clarifies the level of validation, scope, and risks associated with the analysis.
-</text>
   </threadedComment>
   <threadedComment ref="M47" dT="2024-08-29T13:17:16.15" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{94313AA5-1D90-4305-ADF6-5B3D3434DDD2}">
     <text xml:space="preserve">If changes need to be made to any code or analysis, how are these documented? Are changes checked by another member of the team?
@@ -5014,9 +5063,6 @@
   <threadedComment ref="C48" dT="2024-09-02T09:22:26.17" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{213AD9E0-614E-49A3-845F-60CC7100A896}">
     <text>Your analysis must be well documented and repeatable so that somebody new can understand it, use it, and produce the same output with the same inputs. Poor documentation can lead to errors.</text>
   </threadedComment>
-  <threadedComment ref="E48" dT="2024-08-23T10:09:55.54" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D4BC4FCD-085E-4655-8B56-3618CE8762AC}">
-    <text>Good quality analysis is reproducible. Analyst should check that the analytical process reflects the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust)</text>
-  </threadedComment>
   <threadedComment ref="L48" dT="2024-08-29T14:08:39.65" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{94BAB893-D779-406F-A7BF-1CBAB6D2086A}">
     <text xml:space="preserve">Would another analyst be able to pick up from where you left off and reproduce or continue the work (without talking to you first)? </text>
   </threadedComment>
@@ -5028,10 +5074,6 @@
     <text>You should independently review and validate the logical integrity of you analysis as well as the structure and functionality of the code against the research question.
 A record of validation and verification activities undertaken, outstanding tasks and remedial actions helps to confirm that the correct analysis has been performed for the required purpose and the chosen approach minimises risk.</text>
   </threadedComment>
-  <threadedComment ref="E49" dT="2024-08-23T10:10:06.74" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{9635D360-44C4-400F-AB1B-E928C740858A}">
-    <text xml:space="preserve">The analyst should provide proportionate documentation that explains the verification and validation activities that the analysis is subjected to. Analysts must perform appropriate test to check the analysis. They should commission other verification and validation as required. Analytical assurer should confirm that planned validation and verification are sufficient.
-</text>
-  </threadedComment>
   <threadedComment ref="L49" dT="2024-08-29T14:10:04.34" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{BFEC1F1B-CA00-429F-8345-09F20773C97F}">
     <text xml:space="preserve">Do you consistently use peer review to check scripts and code, documentation, implementation of methods, processes and outputs? </text>
   </threadedComment>
@@ -5046,10 +5088,6 @@
   <threadedComment ref="C50" dT="2024-09-02T09:22:52.46" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{3C47F7B2-6A4C-4345-BEDF-BA23749DD7E7}">
     <text>External peer review is one of the best ways to ensure that the analysis and code are well made and fit for purpose. Without it, teams can reinforce their own biases and may not notice there is anything wrong.</text>
   </threadedComment>
-  <threadedComment ref="E50" dT="2024-08-23T10:10:20.22" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B4BE21C7-4D8E-4A10-A05B-7CB29AFCBF11}">
-    <text xml:space="preserve">Analysts should work with the commissioner to set out the analysis question so that appropriate analysis is done. Some analysis may require external specialists, so analysts may have responsibilities as part of the procurement process. Analysts, including 3rd parties providing analysis, should provide proportionate documentation describing the verification and validation activities undertaken and associated conclusions. The analytical assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.
-</text>
-  </threadedComment>
   <threadedComment ref="M50" dT="2024-08-29T13:02:32.78" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{13AD156E-2609-4291-B347-0A9DC3C370C8}">
     <text xml:space="preserve">Is your code or analysis ever peer reviewed by someone outside your team or organisation?
 </text>
@@ -5058,10 +5096,6 @@
     <text xml:space="preserve">Understanding and reporting on the quality of your analysis is critical to ensure fitness for purpose and maintain trust and reliability. This ensures that analysis can appropriately inform decision-making. Quality assessments are key information to share with users and a requirement of the Code of Practice for Statistics.
 </text>
   </threadedComment>
-  <threadedComment ref="E51" dT="2024-08-23T10:10:29.87" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{ECF69508-3E8A-46CC-B588-2FF061AEF2BF}">
-    <text xml:space="preserve">As part of the delivery phase, the commissioner should ensure there is an assessment of the level of analytical quality assurance of the analysis, noting where there have been trade-offs between time, resources and quality. The analytical assurer advises the commissioner on whether appropriate analytical quality assurance has taken place.
-</text>
-  </threadedComment>
   <threadedComment ref="L51" dT="2024-08-29T14:15:45.07" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{2562E7CA-2915-4392-BEB9-1DA6A565E8F7}">
     <text xml:space="preserve">What is the assessment of the quality of your analytical outputs? </text>
   </threadedComment>
@@ -5069,9 +5103,6 @@
     <text xml:space="preserve">If you check that results fit with your expectations and you can explain discrepancies, this makes it easier to mitigate risk.
 There are many ways to check if analysis is carried out correctly. For example, sensitivity analysis can help you understand which inputs have the greatest effect on the outputs. You can also compare figures from the analysis with similar data from other sources or from historical series. </text>
   </threadedComment>
-  <threadedComment ref="E52" dT="2024-08-23T10:10:39.56" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{E240F6D2-DFB8-41B2-967E-7D29D82425D8}">
-    <text>The analyst must build in checks and processes to ensure that the analysis is correct. During the delivery phase, the commissioner should give feedback to assist in the correct interpretation of results and determine if the analysis has addressed the commission. The analyst should work with the analytical assurer while doing the analysis so that they can comment on whether the analysis meets the needs of the commission to ensure best use of the results</text>
-  </threadedComment>
   <threadedComment ref="M52" dT="2024-08-29T13:04:38.41" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{4ED4155D-4BE2-4D08-A20A-46CCE4600A2F}">
     <text xml:space="preserve">How do you assure yourselves that analysis carried out is correct?
 </text>
@@ -5083,16 +5114,10 @@
   <threadedComment ref="C53" dT="2024-09-02T09:23:29.30" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{6E3DB2AC-3774-4582-BCA9-9EFF9F0AAE32}">
     <text>If you can, check that your outputs align with findings from previous runs of the analysis, alternate data sources, and comparable studies. This gives you confidence that the analysis works as expected. You should be able to explain any inconsistencies that you see.</text>
   </threadedComment>
-  <threadedComment ref="E53" dT="2024-08-23T10:10:52.70" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D699B47C-3EDF-439F-9760-748B850EC1F9}">
-    <text>When interpreting the results of a piece of analysis, the commissioner provides constructive challenge. They work with the analyst to explore whether further analysis is needed.</text>
-  </threadedComment>
   <threadedComment ref="C54" dT="2024-09-02T09:23:42.57" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{F15400DE-CFAB-4BA5-8732-2025202D8869}">
     <text xml:space="preserve">It is crucial to check unusual trends and values in the data and understand why they are there. Not all outliers are the same. Some have a strong influence, some not at all. Some are valid and important data values. Others might be errors.
 Investigate outliers and unusual patterns thoroughly and take reasonable steps to check their impact on your final output. If you choose to exclude unusual values, you should explain why this is acceptable. </text>
   </threadedComment>
-  <threadedComment ref="E54" dT="2024-08-23T10:11:03.11" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{FE8BF673-069F-4CC0-85A9-4C68BB190BBB}">
-    <text>If applicable, analyst should undertake parametric analysis to understand the consequences of missing or uncertain data and assumptions. The analysis plan should include treatment of unusual values and outliers. Analytical assurer should be involved.</text>
-  </threadedComment>
   <threadedComment ref="M54" dT="2024-08-29T13:03:43.51" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{FD7F66CA-0ECB-4CE6-B332-6D2FE5F3C81D}">
     <text xml:space="preserve">If you find anomalies or unusual trends in the data, what steps are taken to investigate them?
 </text>
@@ -5100,10 +5125,6 @@
   <threadedComment ref="C55" dT="2024-09-02T09:27:59.56" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{0803AB7E-3746-45D3-A8EA-BDFB8B5C1159}">
     <text>Often the aim of final output is to inform decison-making. Output might include predictions, involving lots of underlying assumptions. It is critical that you support your users to make appropriate use of outputs and understand what can and cannot be inferred. Without this, users may misinterpret findings, make in appropriate comparisons, use the analysis for unsuitable purposes and arrive at the wrong conclusions. For example, a non-expert user may wrongly interpret correlation as causation or use incomplete or disconnected data to make forecasts.</text>
   </threadedComment>
-  <threadedComment ref="E55" dT="2024-08-23T10:25:34.69" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{41424B6F-041D-4E27-8FE0-4FC215D55379}">
-    <text xml:space="preserve">During the delivery phase, the commissioner receives the results of the analysis and decides whether it meets their needs. The analyst provides sufficient information to support the commissioner to make an informed decision.
-</text>
-  </threadedComment>
   <threadedComment ref="L55" dT="2024-08-29T14:11:21.54" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{67623983-4763-4197-A23B-53AA436F8A34}">
     <text xml:space="preserve">Could you give a clear account of what can and cannot be inferred from your analysis or statistical release? </text>
   </threadedComment>
@@ -5114,10 +5135,6 @@
   <threadedComment ref="C56" dT="2024-09-02T09:28:07.62" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{17A37659-8A9C-4B5F-A3EC-709DD0BCE247}">
     <text>You should describe why limitations related to data and methods exist, why they cannot be overcome using the chosen approach and their impact on the quality and interpretation of the output. Analysis is of very little value if limitations aren’t properly documented and explained.</text>
   </threadedComment>
-  <threadedComment ref="E56" dT="2024-08-23T10:25:40.85" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{A926AA69-30D0-40C8-AD64-9B94E4C5EF42}">
-    <text xml:space="preserve">The commissioner must be confident in the quality of the outputs. They should understand the strengths, limitations and context of the analysis so that the results are correctly interpreted. Analytical assurer sign-off provides confidence that analysis risks, limitations and major assumptions are understood by the users of the analysis. Analysts make sure that the commissioner and analytical assurer have the evidence they need.
-</text>
-  </threadedComment>
   <threadedComment ref="L56" dT="2024-08-29T14:10:30.84" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{C2DB1F30-CE98-4E5D-B0C8-B30775816764}">
     <text xml:space="preserve">What are the limitations of your analysis or statistical release? </text>
   </threadedComment>
@@ -5131,35 +5148,18 @@
   <threadedComment ref="C57" dT="2024-09-02T09:28:21.50" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{240D5873-44B0-458F-875A-E4225FD1ACAD}">
     <text>You should work with users, experts, and other relevant stakeholders to verify the credibility of outputs and sense check that they are useful.</text>
   </threadedComment>
-  <threadedComment ref="E57" dT="2024-08-23T10:25:49.48" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B47F104A-FA31-425B-AF50-1422E6F339A4}">
-    <text>The analyst and analytical assurer should enable and encourage peer review. Peer reviews provide useful critical challenge about the analytical approach, application of methods and interpretation of the analysis. Verification and peer review of work should be done by analysts who had no involvement in the work so their views are important.</text>
-  </threadedComment>
   <threadedComment ref="C58" dT="2024-09-02T09:28:32.49" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{DE897266-EE4C-430B-8A06-36671EA1ECF3}">
     <text>Outputs are never 100% accurate. Users need to understand how uncertainties related to data, assumptions and methodology feed into and through the analysis workflow and what this means for the use of the outputs. Results must clearly explain how uncertainty affects the findings from the analysis, or we risk misinterpretations and conclusions being overly reliant on imprecise results.</text>
-  </threadedComment>
-  <threadedComment ref="E58" dT="2024-08-23T10:28:02.88" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{CE50D758-78EF-47CB-8DEF-6F69EB386D92}">
-    <text xml:space="preserve">The analyst must determine and communicate the uncertainty associated with the analysis so the commissioner can make informed decisions. The commissioner should ensure that an assessment of uncertainty has been provided and that the implications of uncertainty are understood.
-</text>
   </threadedComment>
   <threadedComment ref="C59" dT="2024-09-02T09:29:36.72" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D9DCD7D3-EAA6-44D2-9A62-38FD88896CA6}">
     <text xml:space="preserve">You must support your users to understand relevant uncertainties which are not captured in the analysis. When you can, make reasonable judgements about the likely size and direction of unquantified uncertainty. Provide a qualitative description informing users about why the uncertainty cannot be quantified and their likely impact.
 </text>
   </threadedComment>
-  <threadedComment ref="E59" dT="2024-08-23T10:28:09.31" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{057CF385-84BB-476C-8E6A-3FB469600EB4}">
-    <text xml:space="preserve">If uncertainty is too complex to quantify, even approximately, the analysts should explain this so the commissioner can take this into account. In communicating analysis results to decision-makers and stakeholders, the commissioner should be open about the existence of deep uncertainties whose impact cannot be assessed, and explain how they are managed in the analysis.
-</text>
-  </threadedComment>
   <threadedComment ref="C60" dT="2024-09-02T09:29:45.34" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{CF92684F-E55A-4187-96EE-68B56028E8CB}">
     <text>Transparency about your analysis supports proper scrutiny and challenge, promotes public trust, and encourages re-use of the resources you develop.</text>
   </threadedComment>
-  <threadedComment ref="E60" dT="2024-08-23T10:28:15.27" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{D3ECDD38-55DB-42AB-8E24-820D4D27690A}">
-    <text>The analyst must produce appropriate design documentation. Best practice includes maintaining a record of the analysis workflow in a technical report, including a concept of analysis, user requirements, design specification, functional specification, data dictionary, and test plan. Code should be properly documented.</text>
-  </threadedComment>
   <threadedComment ref="C61" dT="2024-09-02T09:29:52.61" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{9626EEC2-270C-466A-BD46-FE28335E7E02}">
     <text>A good technical guide helps everybody to understand what the analysis does and how it works. A well-written technical guide is essential for effective maintenance of the analysis. It helps users of the analysis to replicate the findings, get answers to methodology questions and build their trust in the output.</text>
-  </threadedComment>
-  <threadedComment ref="E61" dT="2024-08-23T10:28:23.58" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{B275DA7B-24DD-46C5-BFD9-1B44FB5FAD46}">
-    <text>The analyst must produce appropriate documentation. Best practice includes maintaining a record of the work that has been done in a technical report, including a full description of the analysis, user requirements, design specification, functional specification, data dictionary, and test plan. The analytical assurer makes sure that the documentation is fit for purpose.</text>
   </threadedComment>
   <threadedComment ref="M61" dT="2024-08-29T13:29:29.13" personId="{5DB4FC9B-6313-426F-8A60-5F9147BC1A6D}" id="{60702B3D-0D4B-4988-B5E8-6A4A2C81D30B}">
     <text xml:space="preserve">How do you ensure that analysis is auditable and can be inspected and understood by colleagues?
@@ -5168,14 +5168,8 @@
   <threadedComment ref="C62" dT="2024-09-02T09:30:24.02" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{6F99AFD3-CF32-4152-A912-1D04F8967B37}">
     <text>The technical guide is complemented by fully documented analysis code. Code documentation must comply with good practice so new users can understand and execute the code as easily and quickly as possible.</text>
   </threadedComment>
-  <threadedComment ref="E62" dT="2024-08-23T10:28:33.13" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{AFF19133-139A-4414-B5BD-D26EEAE944C9}">
-    <text>Analysts should develop and maintain analysis code in line with best practice. Code must comply with relevant policies and standards.</text>
-  </threadedComment>
   <threadedComment ref="C63" dT="2024-09-02T09:30:34.47" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{7DC36BDD-540A-4B1E-9888-76142C106F90}">
     <text xml:space="preserve">External critique makes analysis more robust. Users should be able to give feedback to your team to ensure that results meet their needs. User feedback and customer reviews inform you of issues and changes that you might need to make. They also act as evidence that users have been consulted. </text>
-  </threadedComment>
-  <threadedComment ref="E63" dT="2024-08-23T10:29:21.79" personId="{D56F5C98-9DA8-4D6E-81A2-77932961FFC5}" id="{971985CC-EE2C-4CAC-B5F2-03489CB55C67}">
-    <text>You can assess the usefulness of the analysis by getting feedback from users, stakeholders and other experts. Quality analysis should be free of prejudice or bias. The SRO and analysts should check that the analysis follows the principles of RIGOUR (Repeatable, Independent, Grounded in reality, Objective, Uncertainty-managed, Robust).</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -5252,7 +5246,7 @@
         <v>1.2</v>
       </c>
       <c r="B8" s="104" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>9</v>
@@ -6115,7 +6109,7 @@
     </row>
     <row r="16" spans="1:156" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="53" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="114"/>
@@ -6134,7 +6128,7 @@
     </row>
     <row r="18" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="56" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C18" s="57"/>
       <c r="D18" s="109"/>
@@ -6248,7 +6242,7 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B35" s="50" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C35" s="55"/>
       <c r="D35" s="55"/>
@@ -6256,7 +6250,7 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B36" s="56" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="57"/>
@@ -6316,7 +6310,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6437,7 +6431,7 @@
     </row>
     <row r="3" spans="1:21" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="122" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B3" s="91">
         <v>1</v>
@@ -6446,10 +6440,10 @@
         <v>115</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
@@ -6498,10 +6492,10 @@
         <v>117</v>
       </c>
       <c r="D4" s="92" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E4" s="92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F4" s="68"/>
       <c r="G4" s="68"/>
@@ -6548,7 +6542,7 @@
         <v>118</v>
       </c>
       <c r="D5" s="92" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E5" s="92" t="s">
         <v>90</v>
@@ -6596,10 +6590,10 @@
         <v>119</v>
       </c>
       <c r="D6" s="92" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>195</v>
+        <v>241</v>
       </c>
       <c r="F6" s="68"/>
       <c r="G6" s="68"/>
@@ -6644,10 +6638,10 @@
         <v>120</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E7" s="92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F7" s="68"/>
       <c r="G7" s="68"/>
@@ -6694,10 +6688,10 @@
         <v>121</v>
       </c>
       <c r="D8" s="92" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E8" s="92" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="F8" s="68"/>
       <c r="G8" s="68"/>
@@ -6739,13 +6733,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="92" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F9" s="68"/>
       <c r="G9" s="68"/>
@@ -6789,13 +6783,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="99" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="92" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E10" s="92" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="F10" s="68"/>
       <c r="G10" s="68"/>
@@ -6839,10 +6833,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="99" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D11" s="92" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E11" s="92" t="s">
         <v>90</v>
@@ -6887,13 +6881,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="99" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D12" s="92" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E12" s="92" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F12" s="68"/>
       <c r="G12" s="68"/>
@@ -6935,10 +6929,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="99" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D13" s="92" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E13" s="92" t="s">
         <v>90</v>
@@ -6983,10 +6977,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="99" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D14" s="92" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E14" s="92" t="s">
         <v>90</v>
@@ -7033,10 +7027,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="99" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" s="92" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E15" s="92" t="s">
         <v>90</v>
@@ -7081,13 +7075,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="99" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D16" s="92" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E16" s="92" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="F16" s="68"/>
       <c r="G16" s="68"/>
@@ -7131,13 +7125,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="99" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D17" s="92" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E17" s="92" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F17" s="68"/>
       <c r="G17" s="68"/>
@@ -7179,13 +7173,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="99" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D18" s="92" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -7227,13 +7221,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="99" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D19" s="92" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F19" s="68"/>
       <c r="G19" s="68"/>
@@ -7275,13 +7269,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D20" s="92" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E20" s="92" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="F20" s="68"/>
       <c r="G20" s="68"/>
@@ -7323,13 +7317,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="99" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D21" s="92" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E21" s="92" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="F21" s="68"/>
       <c r="G21" s="68"/>
@@ -7368,20 +7362,20 @@
     </row>
     <row r="22" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="123" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B22" s="93">
         <f>B21+1</f>
         <v>20</v>
       </c>
       <c r="C22" s="100" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D22" s="93" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E22" s="93" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F22" s="73"/>
       <c r="G22" s="73"/>
@@ -7423,13 +7417,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="100" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D23" s="93" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E23" s="93" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F23" s="73"/>
       <c r="G23" s="73"/>
@@ -7475,13 +7469,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="100" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D24" s="93" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="E24" s="93" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F24" s="73"/>
       <c r="G24" s="73"/>
@@ -7525,13 +7519,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D25" s="93" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E25" s="93" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F25" s="73"/>
       <c r="G25" s="73"/>
@@ -7575,13 +7569,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="100" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D26" s="93" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="E26" s="93" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F26" s="73"/>
       <c r="G26" s="73"/>
@@ -7627,13 +7621,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D27" s="93" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E27" s="93" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="F27" s="73"/>
       <c r="G27" s="73"/>
@@ -7672,20 +7666,20 @@
     </row>
     <row r="28" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="124" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B28" s="94">
         <f>B27+1</f>
         <v>26</v>
       </c>
       <c r="C28" s="101" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D28" s="94" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E28" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F28" s="84"/>
       <c r="G28" s="84"/>
@@ -7727,13 +7721,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="101" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D29" s="94" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E29" s="94" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F29" s="84"/>
       <c r="G29" s="84"/>
@@ -7775,13 +7769,13 @@
         <v>28</v>
       </c>
       <c r="C30" s="101" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D30" s="94" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E30" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F30" s="84"/>
       <c r="G30" s="84"/>
@@ -7825,13 +7819,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="101" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D31" s="94" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E31" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F31" s="84"/>
       <c r="G31" s="84"/>
@@ -7875,13 +7869,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="101" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D32" s="94" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E32" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F32" s="84"/>
       <c r="G32" s="84"/>
@@ -7923,13 +7917,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="101" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D33" s="94" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E33" s="94" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F33" s="84"/>
       <c r="G33" s="84"/>
@@ -7973,13 +7967,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="101" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D34" s="94" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E34" s="94" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F34" s="84"/>
       <c r="G34" s="84"/>
@@ -8023,13 +8017,13 @@
         <v>33</v>
       </c>
       <c r="C35" s="101" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D35" s="94" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E35" s="94" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F35" s="84"/>
       <c r="G35" s="84"/>
@@ -8073,13 +8067,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="101" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D36" s="94" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E36" s="94" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F36" s="84"/>
       <c r="G36" s="84"/>
@@ -8123,13 +8117,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="101" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D37" s="94" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E37" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F37" s="84"/>
       <c r="G37" s="84"/>
@@ -8173,13 +8167,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="101" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D38" s="94" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E38" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F38" s="84"/>
       <c r="G38" s="84"/>
@@ -8221,13 +8215,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="101" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D39" s="94" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E39" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F39" s="84"/>
       <c r="G39" s="84"/>
@@ -8273,13 +8267,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="101" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D40" s="94" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E40" s="94" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F40" s="84"/>
       <c r="G40" s="84"/>
@@ -8321,13 +8315,13 @@
         <v>39</v>
       </c>
       <c r="C41" s="101" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D41" s="94" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E41" s="94" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F41" s="84"/>
       <c r="G41" s="84"/>
@@ -8369,13 +8363,13 @@
         <v>40</v>
       </c>
       <c r="C42" s="101" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D42" s="94" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E42" s="94" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F42" s="84"/>
       <c r="G42" s="84"/>
@@ -8419,13 +8413,13 @@
         <v>41</v>
       </c>
       <c r="C43" s="101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D43" s="94" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="E43" s="94" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F43" s="84"/>
       <c r="G43" s="84"/>
@@ -8467,13 +8461,13 @@
         <v>42</v>
       </c>
       <c r="C44" s="101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D44" s="94" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E44" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F44" s="84"/>
       <c r="G44" s="84"/>
@@ -8515,13 +8509,13 @@
         <v>43</v>
       </c>
       <c r="C45" s="101" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D45" s="94" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E45" s="94" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F45" s="84"/>
       <c r="G45" s="84"/>
@@ -8563,13 +8557,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="101" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D46" s="94" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E46" s="94" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F46" s="84"/>
       <c r="G46" s="84"/>
@@ -8611,13 +8605,13 @@
         <v>45</v>
       </c>
       <c r="C47" s="101" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D47" s="94" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E47" s="94" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F47" s="84"/>
       <c r="G47" s="84"/>
@@ -8661,13 +8655,13 @@
         <v>46</v>
       </c>
       <c r="C48" s="101" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" s="94" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E48" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F48" s="84"/>
       <c r="G48" s="84"/>
@@ -8713,13 +8707,13 @@
         <v>47</v>
       </c>
       <c r="C49" s="101" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D49" s="94" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E49" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F49" s="84"/>
       <c r="G49" s="84"/>
@@ -8765,13 +8759,13 @@
         <v>48</v>
       </c>
       <c r="C50" s="101" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D50" s="94" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E50" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F50" s="84"/>
       <c r="G50" s="84"/>
@@ -8815,13 +8809,13 @@
         <v>49</v>
       </c>
       <c r="C51" s="101" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D51" s="94" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E51" s="94" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F51" s="84"/>
       <c r="G51" s="84"/>
@@ -8865,13 +8859,13 @@
         <v>50</v>
       </c>
       <c r="C52" s="101" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D52" s="94" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E52" s="94" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F52" s="84"/>
       <c r="G52" s="84"/>
@@ -8915,13 +8909,13 @@
         <v>51</v>
       </c>
       <c r="C53" s="101" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D53" s="94" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E53" s="94" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F53" s="84"/>
       <c r="G53" s="84"/>
@@ -8963,13 +8957,13 @@
         <v>52</v>
       </c>
       <c r="C54" s="101" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D54" s="94" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E54" s="94" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F54" s="84"/>
       <c r="G54" s="84"/>
@@ -9008,20 +9002,20 @@
     </row>
     <row r="55" spans="1:21" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="117" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B55" s="95">
         <f>B54+1</f>
         <v>53</v>
       </c>
       <c r="C55" s="102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D55" s="95" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E55" s="95" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F55" s="75"/>
       <c r="G55" s="75"/>
@@ -9067,13 +9061,13 @@
         <v>54</v>
       </c>
       <c r="C56" s="102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D56" s="95" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E56" s="95" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F56" s="75"/>
       <c r="G56" s="75"/>
@@ -9119,13 +9113,13 @@
         <v>55</v>
       </c>
       <c r="C57" s="102" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D57" s="95" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E57" s="95" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F57" s="75"/>
       <c r="G57" s="75"/>
@@ -9167,13 +9161,13 @@
         <v>56</v>
       </c>
       <c r="C58" s="102" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D58" s="95" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E58" s="95" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F58" s="75"/>
       <c r="G58" s="75"/>
@@ -9215,13 +9209,13 @@
         <v>57</v>
       </c>
       <c r="C59" s="102" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D59" s="95" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E59" s="95" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F59" s="75"/>
       <c r="G59" s="75"/>
@@ -9263,13 +9257,13 @@
         <v>58</v>
       </c>
       <c r="C60" s="102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D60" s="95" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E60" s="95" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F60" s="75"/>
       <c r="G60" s="75"/>
@@ -9311,13 +9305,13 @@
         <v>59</v>
       </c>
       <c r="C61" s="102" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D61" s="95" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E61" s="95" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F61" s="75"/>
       <c r="G61" s="75"/>
@@ -9361,13 +9355,13 @@
         <v>60</v>
       </c>
       <c r="C62" s="102" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D62" s="95" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E62" s="95" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F62" s="75"/>
       <c r="G62" s="75"/>
@@ -9409,13 +9403,13 @@
         <v>61</v>
       </c>
       <c r="C63" s="102" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D63" s="95" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E63" s="95" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F63" s="75"/>
       <c r="G63" s="75"/>
@@ -9518,7 +9512,7 @@
       <c r="A73" s="81"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="s7nAzo09W2pu2pzQxulB3LlOS7rHZ4SsWO15JFaLskelUu/GN7QvvgWkUmZOUd2ZxrR+liz7CdBg0GlznXakLg==" saltValue="Rbqp9J6mh5Kr1vIR14BXeQ==" spinCount="100000" sheet="1" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0597I8HImh4F9z/A7w2mUw0K3eEHHDpvAvp6XylF25KORn49mFD8b1+7s95xaT6kKXMThkQEMn4QocudbWAIvw==" saltValue="LubhmbeNnYcArVpvOt52lg==" spinCount="100000" sheet="1" autoFilter="0"/>
   <autoFilter ref="A2:U65" xr:uid="{40CE4B58-4DDE-4FFB-AF5D-92EC82F1F313}"/>
   <mergeCells count="6">
     <mergeCell ref="A55:A63"/>
@@ -9528,7 +9522,7 @@
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="A28:A54"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7 L3:L4 M61 L9 M10 M14 M16 M21 M23:M26 L23 L26:L27 L30 M31 M33:M36 L37 L39:M39 L42 M47:M50 L48:L49 L51 M52 M54:M56 L55:L56 M3 N3 O3 O4 N4 N5:N18 O15 P14 P18 O18 N19:N22 O21:O27 P23:P25 Q56 P28:Q29 Q30:Q37 O37:P38 P39 O40:O41 P46 Q25 Q24 T60:T63 S28:S30 R34:S34 R37:S39 S40:S41 R42:S50 T44 R51:S52 S53:S54 R54 T55:T59 R25:R30 R24 U22:U23 U26 U38:U39 U42 U55:U56 U60:U63" xr:uid="{8D995782-9C34-4E27-8832-B7B40AFB5170}">
       <formula1>1</formula1>
     </dataValidation>
@@ -9551,6 +9545,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031C6D98A8BA9914F9CBD1D8D43561C2B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3360ac36c85262295d12999d22c2e363">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e1cd103-0302-4a32-9a4b-e115c950d959" xmlns:ns3="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb3c89d64baff4fee9c4315563c133e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
@@ -9799,7 +9802,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
@@ -9810,16 +9813,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A7238D-7DAD-4EFF-B184-28E2DF4DDCD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E2C66AF-212F-4C93-99E0-4ABA57FC8364}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9838,7 +9840,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85AF8313-FA00-4D59-B28F-14781BE72D64}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
@@ -9855,14 +9857,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A7238D-7DAD-4EFF-B184-28E2DF4DDCD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{078807bf-ce82-4688-bce0-0d811684dc46}" enabled="0" method="" siteId="{078807bf-ce82-4688-bce0-0d811684dc46}" removed="1"/>

</xml_diff>